<commit_message>
James Martinez - Added Naming Rules and Standard Abbreviations tabs
</commit_message>
<xml_diff>
--- a/Reporting_Student_Data_Model_Dictionary.xlsx
+++ b/Reporting_Student_Data_Model_Dictionary.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
+    <sheet name="Naming Rules" sheetId="2" r:id="rId2"/>
+    <sheet name="Standard Abbreviations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5001" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5118" uniqueCount="1145">
   <si>
     <t>Owner</t>
   </si>
@@ -3821,6 +3823,351 @@
       </rPr>
       <t>: WH_F_STU_ENRLMT is a fact table that contains the measures of the section/course enrollment and the grade for the student. The student's primary Academic Career, Academic Program, Academic Plan, Academic Sub Plan, and Degree is included for the term. Surrogate identifiers should be used to joined to dimensions based on how you want to describe the data.</t>
     </r>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Academic</t>
+  </si>
+  <si>
+    <t>ACAD</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>ADDR</t>
+  </si>
+  <si>
+    <t>Advance, Advanced or Advancement</t>
+  </si>
+  <si>
+    <t>ADV</t>
+  </si>
+  <si>
+    <t>Begin or Begining</t>
+  </si>
+  <si>
+    <t>BEG</t>
+  </si>
+  <si>
+    <t>Begin or Begining of Term</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>Biology or Biological</t>
+  </si>
+  <si>
+    <t>BIO</t>
+  </si>
+  <si>
+    <t>Board of Governors</t>
+  </si>
+  <si>
+    <t>BOG</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>Complete or Completion</t>
+  </si>
+  <si>
+    <t>COMPL</t>
+  </si>
+  <si>
+    <t>Cumulative</t>
+  </si>
+  <si>
+    <t>CUM</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>CUR</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>DTTM</t>
+  </si>
+  <si>
+    <t>DESC</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>DIST</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>EDU</t>
+  </si>
+  <si>
+    <t>Effective</t>
+  </si>
+  <si>
+    <t>EFF</t>
+  </si>
+  <si>
+    <t>Effective Date</t>
+  </si>
+  <si>
+    <t>EFFDT</t>
+  </si>
+  <si>
+    <t>Employee Education Program</t>
+  </si>
+  <si>
+    <t>EEP</t>
+  </si>
+  <si>
+    <t>End of Term</t>
+  </si>
+  <si>
+    <t>EOT</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>ENRLMT</t>
+  </si>
+  <si>
+    <t>Formal Description</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>General Education</t>
+  </si>
+  <si>
+    <t>GENED</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Innovation Academy</t>
+  </si>
+  <si>
+    <t>INNOVACAD</t>
+  </si>
+  <si>
+    <t>International</t>
+  </si>
+  <si>
+    <t>INTL</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Long Description</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>Matriculation</t>
+  </si>
+  <si>
+    <t>MATRIC</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>Minium</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>National Student Clearinghouse</t>
+  </si>
+  <si>
+    <t>NSC</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>NUM</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>ORG</t>
+  </si>
+  <si>
+    <t>PeopleSoft</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Percent or Percentage</t>
+  </si>
+  <si>
+    <t>PCT</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>PHYS</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>PROG</t>
+  </si>
+  <si>
+    <t>Required or Requirement</t>
+  </si>
+  <si>
+    <t>REQ</t>
+  </si>
+  <si>
+    <t>Schedule or Scheduled</t>
+  </si>
+  <si>
+    <t>SCHED</t>
+  </si>
+  <si>
+    <t>Science</t>
+  </si>
+  <si>
+    <t>SCI</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>SEQ</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>STU</t>
+  </si>
+  <si>
+    <t>SubPlan</t>
+  </si>
+  <si>
+    <t>SPLAN</t>
+  </si>
+  <si>
+    <t>Surrogate ID</t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>TECH</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>TOT</t>
+  </si>
+  <si>
+    <t>UF Online</t>
+  </si>
+  <si>
+    <t>UFO</t>
+  </si>
+  <si>
+    <t>Every instance of a column containing the same data point will have the same name across all Tables/Views.  Example: ACAD_CAR_CD</t>
+  </si>
+  <si>
+    <t>If a standard abbreviation for a word or phrase exists, that word or phrase will only exist as the abbreviation. Example: ENRLMT (Yes), ENROLLMENT (No)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Words will be seperatated by the underscore character and not run together. Example: EFF_DT (Yes),  EFFDT (No)  </t>
+  </si>
+  <si>
+    <t>Columns names will not contain a "UF_" prefix unless necessary to delineate a UF-owned data point from an identical non UF-owned datapoint in the same Table/View.  Example: UF_GPA, TRANSFER_GPA</t>
+  </si>
+  <si>
+    <t>If a Table/View contains two or more columns containing the same data point, a prefix will be added.  Example: STU_ACAD_CAR_CD, COURSE_ACAD_CAR_CD</t>
+  </si>
+  <si>
+    <t>"FLAG" should be used in place of "INDICATOR" or "IND"</t>
+  </si>
+  <si>
+    <t>We see little value it forcing these "system" column names into compliance, so they  have been retained: SRC_SYS_ID, CREATED_EW_DTTM, LASTUPD_EW_DTTM</t>
   </si>
 </sst>
 </file>
@@ -3920,7 +4267,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3932,18 +4279,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4258,8 +4610,8 @@
   <dimension ref="A1:L1192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1077" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1086" sqref="E1086"/>
+      <pane ySplit="1" topLeftCell="A1113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1131" sqref="D1131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4284,22 +4636,22 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>993</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="2"/>
@@ -4504,39 +4856,39 @@
       <c r="B9" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="12" t="s">
         <v>1000</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
@@ -5562,39 +5914,39 @@
       <c r="B50" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="12" t="s">
         <v>999</v>
       </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D53" s="2"/>
@@ -6056,36 +6408,36 @@
       <c r="L73" s="2"/>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D74" s="8" t="s">
+      <c r="D74" s="12" t="s">
         <v>998</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
     <row r="75" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
@@ -6550,39 +6902,39 @@
       <c r="B95" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D95" s="8" t="s">
+      <c r="D95" s="12" t="s">
         <v>997</v>
       </c>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+      <c r="L95" s="12"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+      <c r="L96" s="12"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
@@ -7094,36 +7446,36 @@
       <c r="L120" s="2"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D121" s="8" t="s">
+      <c r="D121" s="12" t="s">
         <v>996</v>
       </c>
-      <c r="E121" s="8"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
-      <c r="I121" s="8"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12"/>
+      <c r="G121" s="12"/>
+      <c r="H121" s="12"/>
+      <c r="I121" s="12"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
-      <c r="I122" s="8"/>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12"/>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
+      <c r="I122" s="12"/>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8"/>
-      <c r="G123" s="8"/>
-      <c r="H123" s="8"/>
-      <c r="I123" s="8"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="12"/>
+      <c r="H123" s="12"/>
+      <c r="I123" s="12"/>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
@@ -8356,36 +8708,36 @@
       <c r="B173" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D173" s="10" t="s">
+      <c r="D173" s="14" t="s">
         <v>995</v>
       </c>
-      <c r="E173" s="8"/>
-      <c r="F173" s="8"/>
-      <c r="G173" s="8"/>
-      <c r="H173" s="8"/>
-      <c r="I173" s="8"/>
+      <c r="E173" s="12"/>
+      <c r="F173" s="12"/>
+      <c r="G173" s="12"/>
+      <c r="H173" s="12"/>
+      <c r="I173" s="12"/>
       <c r="J173" s="2"/>
       <c r="K173" s="2"/>
       <c r="L173" s="2"/>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D174" s="8"/>
-      <c r="E174" s="8"/>
-      <c r="F174" s="8"/>
-      <c r="G174" s="8"/>
-      <c r="H174" s="8"/>
-      <c r="I174" s="8"/>
+      <c r="D174" s="12"/>
+      <c r="E174" s="12"/>
+      <c r="F174" s="12"/>
+      <c r="G174" s="12"/>
+      <c r="H174" s="12"/>
+      <c r="I174" s="12"/>
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
       <c r="L174" s="2"/>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D175" s="8"/>
-      <c r="E175" s="8"/>
-      <c r="F175" s="8"/>
-      <c r="G175" s="8"/>
-      <c r="H175" s="8"/>
-      <c r="I175" s="8"/>
+      <c r="D175" s="12"/>
+      <c r="E175" s="12"/>
+      <c r="F175" s="12"/>
+      <c r="G175" s="12"/>
+      <c r="H175" s="12"/>
+      <c r="I175" s="12"/>
       <c r="J175" s="2"/>
       <c r="K175" s="2"/>
       <c r="L175" s="2"/>
@@ -9422,36 +9774,36 @@
       <c r="B218" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D218" s="10" t="s">
+      <c r="D218" s="14" t="s">
         <v>994</v>
       </c>
-      <c r="E218" s="8"/>
-      <c r="F218" s="8"/>
-      <c r="G218" s="8"/>
-      <c r="H218" s="8"/>
-      <c r="I218" s="8"/>
+      <c r="E218" s="12"/>
+      <c r="F218" s="12"/>
+      <c r="G218" s="12"/>
+      <c r="H218" s="12"/>
+      <c r="I218" s="12"/>
       <c r="J218" s="2"/>
       <c r="K218" s="2"/>
       <c r="L218" s="2"/>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D219" s="8"/>
-      <c r="E219" s="8"/>
-      <c r="F219" s="8"/>
-      <c r="G219" s="8"/>
-      <c r="H219" s="8"/>
-      <c r="I219" s="8"/>
+      <c r="D219" s="12"/>
+      <c r="E219" s="12"/>
+      <c r="F219" s="12"/>
+      <c r="G219" s="12"/>
+      <c r="H219" s="12"/>
+      <c r="I219" s="12"/>
       <c r="J219" s="2"/>
       <c r="K219" s="2"/>
       <c r="L219" s="2"/>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D220" s="8"/>
-      <c r="E220" s="8"/>
-      <c r="F220" s="8"/>
-      <c r="G220" s="8"/>
-      <c r="H220" s="8"/>
-      <c r="I220" s="8"/>
+      <c r="D220" s="12"/>
+      <c r="E220" s="12"/>
+      <c r="F220" s="12"/>
+      <c r="G220" s="12"/>
+      <c r="H220" s="12"/>
+      <c r="I220" s="12"/>
       <c r="J220" s="2"/>
       <c r="K220" s="2"/>
       <c r="L220" s="2"/>
@@ -10627,36 +10979,36 @@
       <c r="B269" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D269" s="8" t="s">
+      <c r="D269" s="12" t="s">
         <v>1001</v>
       </c>
-      <c r="E269" s="8"/>
-      <c r="F269" s="8"/>
-      <c r="G269" s="8"/>
-      <c r="H269" s="8"/>
-      <c r="I269" s="8"/>
+      <c r="E269" s="12"/>
+      <c r="F269" s="12"/>
+      <c r="G269" s="12"/>
+      <c r="H269" s="12"/>
+      <c r="I269" s="12"/>
       <c r="J269" s="2"/>
       <c r="K269" s="2"/>
       <c r="L269" s="2"/>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D270" s="8"/>
-      <c r="E270" s="8"/>
-      <c r="F270" s="8"/>
-      <c r="G270" s="8"/>
-      <c r="H270" s="8"/>
-      <c r="I270" s="8"/>
+      <c r="D270" s="12"/>
+      <c r="E270" s="12"/>
+      <c r="F270" s="12"/>
+      <c r="G270" s="12"/>
+      <c r="H270" s="12"/>
+      <c r="I270" s="12"/>
       <c r="J270" s="2"/>
       <c r="K270" s="2"/>
       <c r="L270" s="2"/>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D271" s="8"/>
-      <c r="E271" s="8"/>
-      <c r="F271" s="8"/>
-      <c r="G271" s="8"/>
-      <c r="H271" s="8"/>
-      <c r="I271" s="8"/>
+      <c r="D271" s="12"/>
+      <c r="E271" s="12"/>
+      <c r="F271" s="12"/>
+      <c r="G271" s="12"/>
+      <c r="H271" s="12"/>
+      <c r="I271" s="12"/>
       <c r="J271" s="2"/>
       <c r="K271" s="2"/>
       <c r="L271" s="2"/>
@@ -11127,36 +11479,36 @@
       <c r="L291" s="2"/>
     </row>
     <row r="292" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D292" s="12" t="s">
+      <c r="D292" s="13" t="s">
         <v>1002</v>
       </c>
-      <c r="E292" s="12"/>
-      <c r="F292" s="12"/>
-      <c r="G292" s="12"/>
-      <c r="H292" s="12"/>
-      <c r="I292" s="12"/>
+      <c r="E292" s="13"/>
+      <c r="F292" s="13"/>
+      <c r="G292" s="13"/>
+      <c r="H292" s="13"/>
+      <c r="I292" s="13"/>
       <c r="J292" s="2"/>
       <c r="K292" s="2"/>
       <c r="L292" s="2"/>
     </row>
     <row r="293" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D293" s="12"/>
-      <c r="E293" s="12"/>
-      <c r="F293" s="12"/>
-      <c r="G293" s="12"/>
-      <c r="H293" s="12"/>
-      <c r="I293" s="12"/>
+      <c r="D293" s="13"/>
+      <c r="E293" s="13"/>
+      <c r="F293" s="13"/>
+      <c r="G293" s="13"/>
+      <c r="H293" s="13"/>
+      <c r="I293" s="13"/>
       <c r="J293" s="2"/>
       <c r="K293" s="2"/>
       <c r="L293" s="2"/>
     </row>
     <row r="294" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D294" s="12"/>
-      <c r="E294" s="12"/>
-      <c r="F294" s="12"/>
-      <c r="G294" s="12"/>
-      <c r="H294" s="12"/>
-      <c r="I294" s="12"/>
+      <c r="D294" s="13"/>
+      <c r="E294" s="13"/>
+      <c r="F294" s="13"/>
+      <c r="G294" s="13"/>
+      <c r="H294" s="13"/>
+      <c r="I294" s="13"/>
       <c r="J294" s="2"/>
       <c r="K294" s="2"/>
       <c r="L294" s="2"/>
@@ -11481,39 +11833,39 @@
       <c r="B309" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D309" s="8" t="s">
+      <c r="D309" s="12" t="s">
         <v>1003</v>
       </c>
-      <c r="E309" s="8"/>
-      <c r="F309" s="8"/>
-      <c r="G309" s="8"/>
-      <c r="H309" s="8"/>
-      <c r="I309" s="8"/>
-      <c r="J309" s="8"/>
-      <c r="K309" s="8"/>
-      <c r="L309" s="8"/>
+      <c r="E309" s="12"/>
+      <c r="F309" s="12"/>
+      <c r="G309" s="12"/>
+      <c r="H309" s="12"/>
+      <c r="I309" s="12"/>
+      <c r="J309" s="12"/>
+      <c r="K309" s="12"/>
+      <c r="L309" s="12"/>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D310" s="8"/>
-      <c r="E310" s="8"/>
-      <c r="F310" s="8"/>
-      <c r="G310" s="8"/>
-      <c r="H310" s="8"/>
-      <c r="I310" s="8"/>
-      <c r="J310" s="8"/>
-      <c r="K310" s="8"/>
-      <c r="L310" s="8"/>
+      <c r="D310" s="12"/>
+      <c r="E310" s="12"/>
+      <c r="F310" s="12"/>
+      <c r="G310" s="12"/>
+      <c r="H310" s="12"/>
+      <c r="I310" s="12"/>
+      <c r="J310" s="12"/>
+      <c r="K310" s="12"/>
+      <c r="L310" s="12"/>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D311" s="8"/>
-      <c r="E311" s="8"/>
-      <c r="F311" s="8"/>
-      <c r="G311" s="8"/>
-      <c r="H311" s="8"/>
-      <c r="I311" s="8"/>
-      <c r="J311" s="8"/>
-      <c r="K311" s="8"/>
-      <c r="L311" s="8"/>
+      <c r="D311" s="12"/>
+      <c r="E311" s="12"/>
+      <c r="F311" s="12"/>
+      <c r="G311" s="12"/>
+      <c r="H311" s="12"/>
+      <c r="I311" s="12"/>
+      <c r="J311" s="12"/>
+      <c r="K311" s="12"/>
+      <c r="L311" s="12"/>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D312" s="2"/>
@@ -12111,36 +12463,36 @@
       <c r="L336" s="2"/>
     </row>
     <row r="337" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D337" s="12" t="s">
+      <c r="D337" s="13" t="s">
         <v>1004</v>
       </c>
-      <c r="E337" s="12"/>
-      <c r="F337" s="12"/>
-      <c r="G337" s="12"/>
-      <c r="H337" s="12"/>
-      <c r="I337" s="12"/>
+      <c r="E337" s="13"/>
+      <c r="F337" s="13"/>
+      <c r="G337" s="13"/>
+      <c r="H337" s="13"/>
+      <c r="I337" s="13"/>
       <c r="J337" s="2"/>
       <c r="K337" s="2"/>
       <c r="L337" s="2"/>
     </row>
     <row r="338" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D338" s="12"/>
-      <c r="E338" s="12"/>
-      <c r="F338" s="12"/>
-      <c r="G338" s="12"/>
-      <c r="H338" s="12"/>
-      <c r="I338" s="12"/>
+      <c r="D338" s="13"/>
+      <c r="E338" s="13"/>
+      <c r="F338" s="13"/>
+      <c r="G338" s="13"/>
+      <c r="H338" s="13"/>
+      <c r="I338" s="13"/>
       <c r="J338" s="2"/>
       <c r="K338" s="2"/>
       <c r="L338" s="2"/>
     </row>
     <row r="339" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D339" s="12"/>
-      <c r="E339" s="12"/>
-      <c r="F339" s="12"/>
-      <c r="G339" s="12"/>
-      <c r="H339" s="12"/>
-      <c r="I339" s="12"/>
+      <c r="D339" s="13"/>
+      <c r="E339" s="13"/>
+      <c r="F339" s="13"/>
+      <c r="G339" s="13"/>
+      <c r="H339" s="13"/>
+      <c r="I339" s="13"/>
       <c r="J339" s="2"/>
       <c r="K339" s="2"/>
       <c r="L339" s="2"/>
@@ -13851,10 +14203,10 @@
       </c>
     </row>
     <row r="412" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B412" s="14" t="s">
+      <c r="A412" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B412" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C412" s="7" t="s">
@@ -13880,10 +14232,10 @@
       </c>
     </row>
     <row r="413" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A413" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B413" s="14" t="s">
+      <c r="A413" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B413" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C413" s="7" t="s">
@@ -13909,10 +14261,10 @@
       </c>
     </row>
     <row r="414" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A414" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B414" s="14" t="s">
+      <c r="A414" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B414" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C414" s="7" t="s">
@@ -13938,10 +14290,10 @@
       </c>
     </row>
     <row r="415" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A415" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B415" s="14" t="s">
+      <c r="A415" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B415" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C415" s="7" t="s">
@@ -13967,10 +14319,10 @@
       </c>
     </row>
     <row r="416" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A416" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B416" s="14" t="s">
+      <c r="A416" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B416" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C416" s="7" t="s">
@@ -13996,10 +14348,10 @@
       </c>
     </row>
     <row r="417" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A417" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B417" s="14" t="s">
+      <c r="A417" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B417" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C417" s="7" t="s">
@@ -14025,10 +14377,10 @@
       </c>
     </row>
     <row r="418" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A418" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B418" s="14" t="s">
+      <c r="A418" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B418" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C418" s="7" t="s">
@@ -14137,36 +14489,36 @@
       <c r="L422" s="2"/>
     </row>
     <row r="423" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D423" s="12" t="s">
+      <c r="D423" s="13" t="s">
         <v>1005</v>
       </c>
-      <c r="E423" s="12"/>
-      <c r="F423" s="12"/>
-      <c r="G423" s="12"/>
-      <c r="H423" s="12"/>
-      <c r="I423" s="12"/>
+      <c r="E423" s="13"/>
+      <c r="F423" s="13"/>
+      <c r="G423" s="13"/>
+      <c r="H423" s="13"/>
+      <c r="I423" s="13"/>
       <c r="J423" s="2"/>
       <c r="K423" s="2"/>
       <c r="L423" s="2"/>
     </row>
     <row r="424" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D424" s="12"/>
-      <c r="E424" s="12"/>
-      <c r="F424" s="12"/>
-      <c r="G424" s="12"/>
-      <c r="H424" s="12"/>
-      <c r="I424" s="12"/>
+      <c r="D424" s="13"/>
+      <c r="E424" s="13"/>
+      <c r="F424" s="13"/>
+      <c r="G424" s="13"/>
+      <c r="H424" s="13"/>
+      <c r="I424" s="13"/>
       <c r="J424" s="2"/>
       <c r="K424" s="2"/>
       <c r="L424" s="2"/>
     </row>
     <row r="425" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D425" s="12"/>
-      <c r="E425" s="12"/>
-      <c r="F425" s="12"/>
-      <c r="G425" s="12"/>
-      <c r="H425" s="12"/>
-      <c r="I425" s="12"/>
+      <c r="D425" s="13"/>
+      <c r="E425" s="13"/>
+      <c r="F425" s="13"/>
+      <c r="G425" s="13"/>
+      <c r="H425" s="13"/>
+      <c r="I425" s="13"/>
       <c r="J425" s="2"/>
       <c r="K425" s="2"/>
       <c r="L425" s="2"/>
@@ -14461,36 +14813,36 @@
       <c r="L439" s="2"/>
     </row>
     <row r="440" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D440" s="8" t="s">
+      <c r="D440" s="12" t="s">
         <v>1006</v>
       </c>
-      <c r="E440" s="8"/>
-      <c r="F440" s="8"/>
-      <c r="G440" s="8"/>
-      <c r="H440" s="8"/>
-      <c r="I440" s="8"/>
+      <c r="E440" s="12"/>
+      <c r="F440" s="12"/>
+      <c r="G440" s="12"/>
+      <c r="H440" s="12"/>
+      <c r="I440" s="12"/>
       <c r="J440" s="2"/>
       <c r="K440" s="2"/>
       <c r="L440" s="2"/>
     </row>
     <row r="441" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D441" s="8"/>
-      <c r="E441" s="8"/>
-      <c r="F441" s="8"/>
-      <c r="G441" s="8"/>
-      <c r="H441" s="8"/>
-      <c r="I441" s="8"/>
+      <c r="D441" s="12"/>
+      <c r="E441" s="12"/>
+      <c r="F441" s="12"/>
+      <c r="G441" s="12"/>
+      <c r="H441" s="12"/>
+      <c r="I441" s="12"/>
       <c r="J441" s="2"/>
       <c r="K441" s="2"/>
       <c r="L441" s="2"/>
     </row>
     <row r="442" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D442" s="8"/>
-      <c r="E442" s="8"/>
-      <c r="F442" s="8"/>
-      <c r="G442" s="8"/>
-      <c r="H442" s="8"/>
-      <c r="I442" s="8"/>
+      <c r="D442" s="12"/>
+      <c r="E442" s="12"/>
+      <c r="F442" s="12"/>
+      <c r="G442" s="12"/>
+      <c r="H442" s="12"/>
+      <c r="I442" s="12"/>
       <c r="J442" s="2"/>
       <c r="K442" s="2"/>
       <c r="L442" s="2"/>
@@ -14839,36 +15191,36 @@
       <c r="L458" s="2"/>
     </row>
     <row r="459" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D459" s="8" t="s">
+      <c r="D459" s="12" t="s">
         <v>1007</v>
       </c>
-      <c r="E459" s="8"/>
-      <c r="F459" s="8"/>
-      <c r="G459" s="8"/>
-      <c r="H459" s="8"/>
-      <c r="I459" s="8"/>
+      <c r="E459" s="12"/>
+      <c r="F459" s="12"/>
+      <c r="G459" s="12"/>
+      <c r="H459" s="12"/>
+      <c r="I459" s="12"/>
       <c r="J459" s="2"/>
       <c r="K459" s="2"/>
       <c r="L459" s="2"/>
     </row>
     <row r="460" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D460" s="8"/>
-      <c r="E460" s="8"/>
-      <c r="F460" s="8"/>
-      <c r="G460" s="8"/>
-      <c r="H460" s="8"/>
-      <c r="I460" s="8"/>
+      <c r="D460" s="12"/>
+      <c r="E460" s="12"/>
+      <c r="F460" s="12"/>
+      <c r="G460" s="12"/>
+      <c r="H460" s="12"/>
+      <c r="I460" s="12"/>
       <c r="J460" s="2"/>
       <c r="K460" s="2"/>
       <c r="L460" s="2"/>
     </row>
     <row r="461" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D461" s="8"/>
-      <c r="E461" s="8"/>
-      <c r="F461" s="8"/>
-      <c r="G461" s="8"/>
-      <c r="H461" s="8"/>
-      <c r="I461" s="8"/>
+      <c r="D461" s="12"/>
+      <c r="E461" s="12"/>
+      <c r="F461" s="12"/>
+      <c r="G461" s="12"/>
+      <c r="H461" s="12"/>
+      <c r="I461" s="12"/>
       <c r="J461" s="2"/>
       <c r="K461" s="2"/>
       <c r="L461" s="2"/>
@@ -15163,36 +15515,36 @@
       <c r="L475" s="2"/>
     </row>
     <row r="476" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D476" s="8" t="s">
+      <c r="D476" s="12" t="s">
         <v>1008</v>
       </c>
-      <c r="E476" s="8"/>
-      <c r="F476" s="8"/>
-      <c r="G476" s="8"/>
-      <c r="H476" s="8"/>
-      <c r="I476" s="8"/>
+      <c r="E476" s="12"/>
+      <c r="F476" s="12"/>
+      <c r="G476" s="12"/>
+      <c r="H476" s="12"/>
+      <c r="I476" s="12"/>
       <c r="J476" s="2"/>
       <c r="K476" s="2"/>
       <c r="L476" s="2"/>
     </row>
     <row r="477" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D477" s="8"/>
-      <c r="E477" s="8"/>
-      <c r="F477" s="8"/>
-      <c r="G477" s="8"/>
-      <c r="H477" s="8"/>
-      <c r="I477" s="8"/>
+      <c r="D477" s="12"/>
+      <c r="E477" s="12"/>
+      <c r="F477" s="12"/>
+      <c r="G477" s="12"/>
+      <c r="H477" s="12"/>
+      <c r="I477" s="12"/>
       <c r="J477" s="2"/>
       <c r="K477" s="2"/>
       <c r="L477" s="2"/>
     </row>
     <row r="478" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D478" s="8"/>
-      <c r="E478" s="8"/>
-      <c r="F478" s="8"/>
-      <c r="G478" s="8"/>
-      <c r="H478" s="8"/>
-      <c r="I478" s="8"/>
+      <c r="D478" s="12"/>
+      <c r="E478" s="12"/>
+      <c r="F478" s="12"/>
+      <c r="G478" s="12"/>
+      <c r="H478" s="12"/>
+      <c r="I478" s="12"/>
       <c r="J478" s="2"/>
       <c r="K478" s="2"/>
       <c r="L478" s="2"/>
@@ -15573,39 +15925,39 @@
       <c r="B495" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D495" s="8" t="s">
+      <c r="D495" s="12" t="s">
         <v>1009</v>
       </c>
-      <c r="E495" s="8"/>
-      <c r="F495" s="8"/>
-      <c r="G495" s="8"/>
-      <c r="H495" s="8"/>
-      <c r="I495" s="8"/>
-      <c r="J495" s="8"/>
-      <c r="K495" s="8"/>
-      <c r="L495" s="8"/>
+      <c r="E495" s="12"/>
+      <c r="F495" s="12"/>
+      <c r="G495" s="12"/>
+      <c r="H495" s="12"/>
+      <c r="I495" s="12"/>
+      <c r="J495" s="12"/>
+      <c r="K495" s="12"/>
+      <c r="L495" s="12"/>
     </row>
     <row r="496" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D496" s="8"/>
-      <c r="E496" s="8"/>
-      <c r="F496" s="8"/>
-      <c r="G496" s="8"/>
-      <c r="H496" s="8"/>
-      <c r="I496" s="8"/>
-      <c r="J496" s="8"/>
-      <c r="K496" s="8"/>
-      <c r="L496" s="8"/>
+      <c r="D496" s="12"/>
+      <c r="E496" s="12"/>
+      <c r="F496" s="12"/>
+      <c r="G496" s="12"/>
+      <c r="H496" s="12"/>
+      <c r="I496" s="12"/>
+      <c r="J496" s="12"/>
+      <c r="K496" s="12"/>
+      <c r="L496" s="12"/>
     </row>
     <row r="497" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D497" s="8"/>
-      <c r="E497" s="8"/>
-      <c r="F497" s="8"/>
-      <c r="G497" s="8"/>
-      <c r="H497" s="8"/>
-      <c r="I497" s="8"/>
-      <c r="J497" s="8"/>
-      <c r="K497" s="8"/>
-      <c r="L497" s="8"/>
+      <c r="D497" s="12"/>
+      <c r="E497" s="12"/>
+      <c r="F497" s="12"/>
+      <c r="G497" s="12"/>
+      <c r="H497" s="12"/>
+      <c r="I497" s="12"/>
+      <c r="J497" s="12"/>
+      <c r="K497" s="12"/>
+      <c r="L497" s="12"/>
     </row>
     <row r="498" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D498" s="2"/>
@@ -16185,36 +16537,36 @@
       <c r="L521" s="2"/>
     </row>
     <row r="522" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D522" s="8" t="s">
+      <c r="D522" s="12" t="s">
         <v>1010</v>
       </c>
-      <c r="E522" s="8"/>
-      <c r="F522" s="8"/>
-      <c r="G522" s="8"/>
-      <c r="H522" s="8"/>
-      <c r="I522" s="8"/>
+      <c r="E522" s="12"/>
+      <c r="F522" s="12"/>
+      <c r="G522" s="12"/>
+      <c r="H522" s="12"/>
+      <c r="I522" s="12"/>
       <c r="J522" s="2"/>
       <c r="K522" s="2"/>
       <c r="L522" s="2"/>
     </row>
     <row r="523" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D523" s="8"/>
-      <c r="E523" s="8"/>
-      <c r="F523" s="8"/>
-      <c r="G523" s="8"/>
-      <c r="H523" s="8"/>
-      <c r="I523" s="8"/>
+      <c r="D523" s="12"/>
+      <c r="E523" s="12"/>
+      <c r="F523" s="12"/>
+      <c r="G523" s="12"/>
+      <c r="H523" s="12"/>
+      <c r="I523" s="12"/>
       <c r="J523" s="2"/>
       <c r="K523" s="2"/>
       <c r="L523" s="2"/>
     </row>
     <row r="524" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D524" s="8"/>
-      <c r="E524" s="8"/>
-      <c r="F524" s="8"/>
-      <c r="G524" s="8"/>
-      <c r="H524" s="8"/>
-      <c r="I524" s="8"/>
+      <c r="D524" s="12"/>
+      <c r="E524" s="12"/>
+      <c r="F524" s="12"/>
+      <c r="G524" s="12"/>
+      <c r="H524" s="12"/>
+      <c r="I524" s="12"/>
       <c r="J524" s="2"/>
       <c r="K524" s="2"/>
       <c r="L524" s="2"/>
@@ -17097,69 +17449,69 @@
       <c r="L560" s="2"/>
     </row>
     <row r="561" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D561" s="8" t="s">
+      <c r="D561" s="12" t="s">
         <v>1011</v>
       </c>
-      <c r="E561" s="8"/>
-      <c r="F561" s="8"/>
-      <c r="G561" s="8"/>
-      <c r="H561" s="8"/>
-      <c r="I561" s="8"/>
+      <c r="E561" s="12"/>
+      <c r="F561" s="12"/>
+      <c r="G561" s="12"/>
+      <c r="H561" s="12"/>
+      <c r="I561" s="12"/>
       <c r="J561" s="2"/>
       <c r="K561" s="2"/>
       <c r="L561" s="2"/>
     </row>
     <row r="562" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D562" s="8"/>
-      <c r="E562" s="8"/>
-      <c r="F562" s="8"/>
-      <c r="G562" s="8"/>
-      <c r="H562" s="8"/>
-      <c r="I562" s="8"/>
+      <c r="D562" s="12"/>
+      <c r="E562" s="12"/>
+      <c r="F562" s="12"/>
+      <c r="G562" s="12"/>
+      <c r="H562" s="12"/>
+      <c r="I562" s="12"/>
       <c r="J562" s="2"/>
       <c r="K562" s="2"/>
       <c r="L562" s="2"/>
     </row>
     <row r="563" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D563" s="8"/>
-      <c r="E563" s="8"/>
-      <c r="F563" s="8"/>
-      <c r="G563" s="8"/>
-      <c r="H563" s="8"/>
-      <c r="I563" s="8"/>
+      <c r="D563" s="12"/>
+      <c r="E563" s="12"/>
+      <c r="F563" s="12"/>
+      <c r="G563" s="12"/>
+      <c r="H563" s="12"/>
+      <c r="I563" s="12"/>
       <c r="J563" s="2"/>
       <c r="K563" s="2"/>
       <c r="L563" s="2"/>
     </row>
     <row r="564" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D564" s="9"/>
-      <c r="E564" s="9"/>
-      <c r="F564" s="9"/>
-      <c r="G564" s="9"/>
-      <c r="H564" s="9"/>
-      <c r="I564" s="9"/>
+      <c r="D564" s="8"/>
+      <c r="E564" s="8"/>
+      <c r="F564" s="8"/>
+      <c r="G564" s="8"/>
+      <c r="H564" s="8"/>
+      <c r="I564" s="8"/>
       <c r="J564" s="2"/>
       <c r="K564" s="2"/>
       <c r="L564" s="2"/>
     </row>
     <row r="565" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D565" s="9"/>
-      <c r="E565" s="9"/>
-      <c r="F565" s="9"/>
-      <c r="G565" s="9"/>
-      <c r="H565" s="9"/>
-      <c r="I565" s="9"/>
+      <c r="D565" s="8"/>
+      <c r="E565" s="8"/>
+      <c r="F565" s="8"/>
+      <c r="G565" s="8"/>
+      <c r="H565" s="8"/>
+      <c r="I565" s="8"/>
       <c r="J565" s="2"/>
       <c r="K565" s="2"/>
       <c r="L565" s="2"/>
     </row>
     <row r="566" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D566" s="9"/>
-      <c r="E566" s="9"/>
-      <c r="F566" s="9"/>
-      <c r="G566" s="9"/>
-      <c r="H566" s="9"/>
-      <c r="I566" s="9"/>
+      <c r="D566" s="8"/>
+      <c r="E566" s="8"/>
+      <c r="F566" s="8"/>
+      <c r="G566" s="8"/>
+      <c r="H566" s="8"/>
+      <c r="I566" s="8"/>
       <c r="J566" s="2"/>
       <c r="K566" s="2"/>
       <c r="L566" s="2"/>
@@ -17237,36 +17589,36 @@
       <c r="L570" s="2"/>
     </row>
     <row r="571" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D571" s="8" t="s">
+      <c r="D571" s="12" t="s">
         <v>1012</v>
       </c>
-      <c r="E571" s="8"/>
-      <c r="F571" s="8"/>
-      <c r="G571" s="8"/>
-      <c r="H571" s="8"/>
-      <c r="I571" s="8"/>
+      <c r="E571" s="12"/>
+      <c r="F571" s="12"/>
+      <c r="G571" s="12"/>
+      <c r="H571" s="12"/>
+      <c r="I571" s="12"/>
       <c r="J571" s="2"/>
       <c r="K571" s="2"/>
       <c r="L571" s="2"/>
     </row>
     <row r="572" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D572" s="8"/>
-      <c r="E572" s="8"/>
-      <c r="F572" s="8"/>
-      <c r="G572" s="8"/>
-      <c r="H572" s="8"/>
-      <c r="I572" s="8"/>
+      <c r="D572" s="12"/>
+      <c r="E572" s="12"/>
+      <c r="F572" s="12"/>
+      <c r="G572" s="12"/>
+      <c r="H572" s="12"/>
+      <c r="I572" s="12"/>
       <c r="J572" s="2"/>
       <c r="K572" s="2"/>
       <c r="L572" s="2"/>
     </row>
     <row r="573" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D573" s="8"/>
-      <c r="E573" s="8"/>
-      <c r="F573" s="8"/>
-      <c r="G573" s="8"/>
-      <c r="H573" s="8"/>
-      <c r="I573" s="8"/>
+      <c r="D573" s="12"/>
+      <c r="E573" s="12"/>
+      <c r="F573" s="12"/>
+      <c r="G573" s="12"/>
+      <c r="H573" s="12"/>
+      <c r="I573" s="12"/>
       <c r="J573" s="2"/>
       <c r="K573" s="2"/>
       <c r="L573" s="2"/>
@@ -17550,36 +17902,36 @@
       <c r="L586" s="2"/>
     </row>
     <row r="587" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D587" s="8" t="s">
+      <c r="D587" s="12" t="s">
         <v>1013</v>
       </c>
-      <c r="E587" s="8"/>
-      <c r="F587" s="8"/>
-      <c r="G587" s="8"/>
-      <c r="H587" s="8"/>
-      <c r="I587" s="8"/>
+      <c r="E587" s="12"/>
+      <c r="F587" s="12"/>
+      <c r="G587" s="12"/>
+      <c r="H587" s="12"/>
+      <c r="I587" s="12"/>
       <c r="J587" s="2"/>
       <c r="K587" s="2"/>
       <c r="L587" s="2"/>
     </row>
     <row r="588" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D588" s="8"/>
-      <c r="E588" s="8"/>
-      <c r="F588" s="8"/>
-      <c r="G588" s="8"/>
-      <c r="H588" s="8"/>
-      <c r="I588" s="8"/>
+      <c r="D588" s="12"/>
+      <c r="E588" s="12"/>
+      <c r="F588" s="12"/>
+      <c r="G588" s="12"/>
+      <c r="H588" s="12"/>
+      <c r="I588" s="12"/>
       <c r="J588" s="2"/>
       <c r="K588" s="2"/>
       <c r="L588" s="2"/>
     </row>
     <row r="589" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D589" s="8"/>
-      <c r="E589" s="8"/>
-      <c r="F589" s="8"/>
-      <c r="G589" s="8"/>
-      <c r="H589" s="8"/>
-      <c r="I589" s="8"/>
+      <c r="D589" s="12"/>
+      <c r="E589" s="12"/>
+      <c r="F589" s="12"/>
+      <c r="G589" s="12"/>
+      <c r="H589" s="12"/>
+      <c r="I589" s="12"/>
       <c r="J589" s="2"/>
       <c r="K589" s="2"/>
       <c r="L589" s="2"/>
@@ -17931,36 +18283,36 @@
       <c r="L605" s="2"/>
     </row>
     <row r="606" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D606" s="8" t="s">
+      <c r="D606" s="12" t="s">
         <v>1014</v>
       </c>
-      <c r="E606" s="8"/>
-      <c r="F606" s="8"/>
-      <c r="G606" s="8"/>
-      <c r="H606" s="8"/>
-      <c r="I606" s="8"/>
+      <c r="E606" s="12"/>
+      <c r="F606" s="12"/>
+      <c r="G606" s="12"/>
+      <c r="H606" s="12"/>
+      <c r="I606" s="12"/>
       <c r="J606" s="2"/>
       <c r="K606" s="2"/>
       <c r="L606" s="2"/>
     </row>
     <row r="607" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D607" s="8"/>
-      <c r="E607" s="8"/>
-      <c r="F607" s="8"/>
-      <c r="G607" s="8"/>
-      <c r="H607" s="8"/>
-      <c r="I607" s="8"/>
+      <c r="D607" s="12"/>
+      <c r="E607" s="12"/>
+      <c r="F607" s="12"/>
+      <c r="G607" s="12"/>
+      <c r="H607" s="12"/>
+      <c r="I607" s="12"/>
       <c r="J607" s="2"/>
       <c r="K607" s="2"/>
       <c r="L607" s="2"/>
     </row>
     <row r="608" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D608" s="8"/>
-      <c r="E608" s="8"/>
-      <c r="F608" s="8"/>
-      <c r="G608" s="8"/>
-      <c r="H608" s="8"/>
-      <c r="I608" s="8"/>
+      <c r="D608" s="12"/>
+      <c r="E608" s="12"/>
+      <c r="F608" s="12"/>
+      <c r="G608" s="12"/>
+      <c r="H608" s="12"/>
+      <c r="I608" s="12"/>
       <c r="J608" s="2"/>
       <c r="K608" s="2"/>
       <c r="L608" s="2"/>
@@ -18252,36 +18604,36 @@
       <c r="L622" s="2"/>
     </row>
     <row r="623" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D623" s="8" t="s">
+      <c r="D623" s="12" t="s">
         <v>1015</v>
       </c>
-      <c r="E623" s="8"/>
-      <c r="F623" s="8"/>
-      <c r="G623" s="8"/>
-      <c r="H623" s="8"/>
-      <c r="I623" s="8"/>
+      <c r="E623" s="12"/>
+      <c r="F623" s="12"/>
+      <c r="G623" s="12"/>
+      <c r="H623" s="12"/>
+      <c r="I623" s="12"/>
       <c r="J623" s="2"/>
       <c r="K623" s="2"/>
       <c r="L623" s="2"/>
     </row>
     <row r="624" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D624" s="8"/>
-      <c r="E624" s="8"/>
-      <c r="F624" s="8"/>
-      <c r="G624" s="8"/>
-      <c r="H624" s="8"/>
-      <c r="I624" s="8"/>
+      <c r="D624" s="12"/>
+      <c r="E624" s="12"/>
+      <c r="F624" s="12"/>
+      <c r="G624" s="12"/>
+      <c r="H624" s="12"/>
+      <c r="I624" s="12"/>
       <c r="J624" s="2"/>
       <c r="K624" s="2"/>
       <c r="L624" s="2"/>
     </row>
     <row r="625" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D625" s="8"/>
-      <c r="E625" s="8"/>
-      <c r="F625" s="8"/>
-      <c r="G625" s="8"/>
-      <c r="H625" s="8"/>
-      <c r="I625" s="8"/>
+      <c r="D625" s="12"/>
+      <c r="E625" s="12"/>
+      <c r="F625" s="12"/>
+      <c r="G625" s="12"/>
+      <c r="H625" s="12"/>
+      <c r="I625" s="12"/>
       <c r="J625" s="2"/>
       <c r="K625" s="2"/>
       <c r="L625" s="2"/>
@@ -18846,36 +19198,36 @@
       <c r="L650" s="2"/>
     </row>
     <row r="651" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D651" s="8" t="s">
+      <c r="D651" s="12" t="s">
         <v>1016</v>
       </c>
-      <c r="E651" s="8"/>
-      <c r="F651" s="8"/>
-      <c r="G651" s="8"/>
-      <c r="H651" s="8"/>
-      <c r="I651" s="8"/>
+      <c r="E651" s="12"/>
+      <c r="F651" s="12"/>
+      <c r="G651" s="12"/>
+      <c r="H651" s="12"/>
+      <c r="I651" s="12"/>
       <c r="J651" s="2"/>
       <c r="K651" s="2"/>
       <c r="L651" s="2"/>
     </row>
     <row r="652" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D652" s="8"/>
-      <c r="E652" s="8"/>
-      <c r="F652" s="8"/>
-      <c r="G652" s="8"/>
-      <c r="H652" s="8"/>
-      <c r="I652" s="8"/>
+      <c r="D652" s="12"/>
+      <c r="E652" s="12"/>
+      <c r="F652" s="12"/>
+      <c r="G652" s="12"/>
+      <c r="H652" s="12"/>
+      <c r="I652" s="12"/>
       <c r="J652" s="2"/>
       <c r="K652" s="2"/>
       <c r="L652" s="2"/>
     </row>
     <row r="653" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D653" s="8"/>
-      <c r="E653" s="8"/>
-      <c r="F653" s="8"/>
-      <c r="G653" s="8"/>
-      <c r="H653" s="8"/>
-      <c r="I653" s="8"/>
+      <c r="D653" s="12"/>
+      <c r="E653" s="12"/>
+      <c r="F653" s="12"/>
+      <c r="G653" s="12"/>
+      <c r="H653" s="12"/>
+      <c r="I653" s="12"/>
       <c r="J653" s="2"/>
       <c r="K653" s="2"/>
       <c r="L653" s="2"/>
@@ -22592,36 +22944,36 @@
       <c r="L788" s="2"/>
     </row>
     <row r="789" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D789" s="8" t="s">
+      <c r="D789" s="12" t="s">
         <v>1017</v>
       </c>
-      <c r="E789" s="8"/>
-      <c r="F789" s="8"/>
-      <c r="G789" s="8"/>
-      <c r="H789" s="8"/>
-      <c r="I789" s="8"/>
+      <c r="E789" s="12"/>
+      <c r="F789" s="12"/>
+      <c r="G789" s="12"/>
+      <c r="H789" s="12"/>
+      <c r="I789" s="12"/>
       <c r="J789" s="2"/>
       <c r="K789" s="2"/>
       <c r="L789" s="2"/>
     </row>
     <row r="790" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D790" s="8"/>
-      <c r="E790" s="8"/>
-      <c r="F790" s="8"/>
-      <c r="G790" s="8"/>
-      <c r="H790" s="8"/>
-      <c r="I790" s="8"/>
+      <c r="D790" s="12"/>
+      <c r="E790" s="12"/>
+      <c r="F790" s="12"/>
+      <c r="G790" s="12"/>
+      <c r="H790" s="12"/>
+      <c r="I790" s="12"/>
       <c r="J790" s="2"/>
       <c r="K790" s="2"/>
       <c r="L790" s="2"/>
     </row>
     <row r="791" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D791" s="8"/>
-      <c r="E791" s="8"/>
-      <c r="F791" s="8"/>
-      <c r="G791" s="8"/>
-      <c r="H791" s="8"/>
-      <c r="I791" s="8"/>
+      <c r="D791" s="12"/>
+      <c r="E791" s="12"/>
+      <c r="F791" s="12"/>
+      <c r="G791" s="12"/>
+      <c r="H791" s="12"/>
+      <c r="I791" s="12"/>
       <c r="J791" s="2"/>
       <c r="K791" s="2"/>
       <c r="L791" s="2"/>
@@ -24135,39 +24487,39 @@
       <c r="B849" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D849" s="8" t="s">
+      <c r="D849" s="12" t="s">
         <v>1018</v>
       </c>
-      <c r="E849" s="8"/>
-      <c r="F849" s="8"/>
-      <c r="G849" s="8"/>
-      <c r="H849" s="8"/>
-      <c r="I849" s="8"/>
-      <c r="J849" s="8"/>
-      <c r="K849" s="8"/>
-      <c r="L849" s="8"/>
+      <c r="E849" s="12"/>
+      <c r="F849" s="12"/>
+      <c r="G849" s="12"/>
+      <c r="H849" s="12"/>
+      <c r="I849" s="12"/>
+      <c r="J849" s="12"/>
+      <c r="K849" s="12"/>
+      <c r="L849" s="12"/>
     </row>
     <row r="850" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D850" s="8"/>
-      <c r="E850" s="8"/>
-      <c r="F850" s="8"/>
-      <c r="G850" s="8"/>
-      <c r="H850" s="8"/>
-      <c r="I850" s="8"/>
-      <c r="J850" s="8"/>
-      <c r="K850" s="8"/>
-      <c r="L850" s="8"/>
+      <c r="D850" s="12"/>
+      <c r="E850" s="12"/>
+      <c r="F850" s="12"/>
+      <c r="G850" s="12"/>
+      <c r="H850" s="12"/>
+      <c r="I850" s="12"/>
+      <c r="J850" s="12"/>
+      <c r="K850" s="12"/>
+      <c r="L850" s="12"/>
     </row>
     <row r="851" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D851" s="8"/>
-      <c r="E851" s="8"/>
-      <c r="F851" s="8"/>
-      <c r="G851" s="8"/>
-      <c r="H851" s="8"/>
-      <c r="I851" s="8"/>
-      <c r="J851" s="8"/>
-      <c r="K851" s="8"/>
-      <c r="L851" s="8"/>
+      <c r="D851" s="12"/>
+      <c r="E851" s="12"/>
+      <c r="F851" s="12"/>
+      <c r="G851" s="12"/>
+      <c r="H851" s="12"/>
+      <c r="I851" s="12"/>
+      <c r="J851" s="12"/>
+      <c r="K851" s="12"/>
+      <c r="L851" s="12"/>
     </row>
     <row r="852" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D852" s="2"/>
@@ -24484,39 +24836,39 @@
       <c r="B866" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D866" s="8" t="s">
+      <c r="D866" s="12" t="s">
         <v>1019</v>
       </c>
-      <c r="E866" s="8"/>
-      <c r="F866" s="8"/>
-      <c r="G866" s="8"/>
-      <c r="H866" s="8"/>
-      <c r="I866" s="8"/>
-      <c r="J866" s="8"/>
-      <c r="K866" s="8"/>
-      <c r="L866" s="8"/>
+      <c r="E866" s="12"/>
+      <c r="F866" s="12"/>
+      <c r="G866" s="12"/>
+      <c r="H866" s="12"/>
+      <c r="I866" s="12"/>
+      <c r="J866" s="12"/>
+      <c r="K866" s="12"/>
+      <c r="L866" s="12"/>
     </row>
     <row r="867" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D867" s="8"/>
-      <c r="E867" s="8"/>
-      <c r="F867" s="8"/>
-      <c r="G867" s="8"/>
-      <c r="H867" s="8"/>
-      <c r="I867" s="8"/>
-      <c r="J867" s="8"/>
-      <c r="K867" s="8"/>
-      <c r="L867" s="8"/>
+      <c r="D867" s="12"/>
+      <c r="E867" s="12"/>
+      <c r="F867" s="12"/>
+      <c r="G867" s="12"/>
+      <c r="H867" s="12"/>
+      <c r="I867" s="12"/>
+      <c r="J867" s="12"/>
+      <c r="K867" s="12"/>
+      <c r="L867" s="12"/>
     </row>
     <row r="868" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D868" s="8"/>
-      <c r="E868" s="8"/>
-      <c r="F868" s="8"/>
-      <c r="G868" s="8"/>
-      <c r="H868" s="8"/>
-      <c r="I868" s="8"/>
-      <c r="J868" s="8"/>
-      <c r="K868" s="8"/>
-      <c r="L868" s="8"/>
+      <c r="D868" s="12"/>
+      <c r="E868" s="12"/>
+      <c r="F868" s="12"/>
+      <c r="G868" s="12"/>
+      <c r="H868" s="12"/>
+      <c r="I868" s="12"/>
+      <c r="J868" s="12"/>
+      <c r="K868" s="12"/>
+      <c r="L868" s="12"/>
     </row>
     <row r="869" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D869" s="2"/>
@@ -24833,39 +25185,39 @@
       <c r="B883" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D883" s="8" t="s">
+      <c r="D883" s="12" t="s">
         <v>1020</v>
       </c>
-      <c r="E883" s="8"/>
-      <c r="F883" s="8"/>
-      <c r="G883" s="8"/>
-      <c r="H883" s="8"/>
-      <c r="I883" s="8"/>
-      <c r="J883" s="8"/>
-      <c r="K883" s="8"/>
-      <c r="L883" s="8"/>
+      <c r="E883" s="12"/>
+      <c r="F883" s="12"/>
+      <c r="G883" s="12"/>
+      <c r="H883" s="12"/>
+      <c r="I883" s="12"/>
+      <c r="J883" s="12"/>
+      <c r="K883" s="12"/>
+      <c r="L883" s="12"/>
     </row>
     <row r="884" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D884" s="8"/>
-      <c r="E884" s="8"/>
-      <c r="F884" s="8"/>
-      <c r="G884" s="8"/>
-      <c r="H884" s="8"/>
-      <c r="I884" s="8"/>
-      <c r="J884" s="8"/>
-      <c r="K884" s="8"/>
-      <c r="L884" s="8"/>
+      <c r="D884" s="12"/>
+      <c r="E884" s="12"/>
+      <c r="F884" s="12"/>
+      <c r="G884" s="12"/>
+      <c r="H884" s="12"/>
+      <c r="I884" s="12"/>
+      <c r="J884" s="12"/>
+      <c r="K884" s="12"/>
+      <c r="L884" s="12"/>
     </row>
     <row r="885" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D885" s="8"/>
-      <c r="E885" s="8"/>
-      <c r="F885" s="8"/>
-      <c r="G885" s="8"/>
-      <c r="H885" s="8"/>
-      <c r="I885" s="8"/>
-      <c r="J885" s="8"/>
-      <c r="K885" s="8"/>
-      <c r="L885" s="8"/>
+      <c r="D885" s="12"/>
+      <c r="E885" s="12"/>
+      <c r="F885" s="12"/>
+      <c r="G885" s="12"/>
+      <c r="H885" s="12"/>
+      <c r="I885" s="12"/>
+      <c r="J885" s="12"/>
+      <c r="K885" s="12"/>
+      <c r="L885" s="12"/>
     </row>
     <row r="886" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D886" s="2"/>
@@ -25479,36 +25831,36 @@
       <c r="B912" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D912" s="8" t="s">
+      <c r="D912" s="12" t="s">
         <v>1021</v>
       </c>
-      <c r="E912" s="8"/>
-      <c r="F912" s="8"/>
-      <c r="G912" s="8"/>
-      <c r="H912" s="8"/>
-      <c r="I912" s="8"/>
+      <c r="E912" s="12"/>
+      <c r="F912" s="12"/>
+      <c r="G912" s="12"/>
+      <c r="H912" s="12"/>
+      <c r="I912" s="12"/>
       <c r="J912" s="2"/>
       <c r="K912" s="2"/>
       <c r="L912" s="2"/>
     </row>
     <row r="913" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D913" s="8"/>
-      <c r="E913" s="8"/>
-      <c r="F913" s="8"/>
-      <c r="G913" s="8"/>
-      <c r="H913" s="8"/>
-      <c r="I913" s="8"/>
+      <c r="D913" s="12"/>
+      <c r="E913" s="12"/>
+      <c r="F913" s="12"/>
+      <c r="G913" s="12"/>
+      <c r="H913" s="12"/>
+      <c r="I913" s="12"/>
       <c r="J913" s="2"/>
       <c r="K913" s="2"/>
       <c r="L913" s="2"/>
     </row>
     <row r="914" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D914" s="8"/>
-      <c r="E914" s="8"/>
-      <c r="F914" s="8"/>
-      <c r="G914" s="8"/>
-      <c r="H914" s="8"/>
-      <c r="I914" s="8"/>
+      <c r="D914" s="12"/>
+      <c r="E914" s="12"/>
+      <c r="F914" s="12"/>
+      <c r="G914" s="12"/>
+      <c r="H914" s="12"/>
+      <c r="I914" s="12"/>
       <c r="J914" s="2"/>
       <c r="K914" s="2"/>
       <c r="L914" s="2"/>
@@ -25922,36 +26274,36 @@
       <c r="L932" s="2"/>
     </row>
     <row r="933" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D933" s="8" t="s">
+      <c r="D933" s="12" t="s">
         <v>1022</v>
       </c>
-      <c r="E933" s="8"/>
-      <c r="F933" s="8"/>
-      <c r="G933" s="8"/>
-      <c r="H933" s="8"/>
-      <c r="I933" s="8"/>
+      <c r="E933" s="12"/>
+      <c r="F933" s="12"/>
+      <c r="G933" s="12"/>
+      <c r="H933" s="12"/>
+      <c r="I933" s="12"/>
       <c r="J933" s="2"/>
       <c r="K933" s="2"/>
       <c r="L933" s="2"/>
     </row>
     <row r="934" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D934" s="8"/>
-      <c r="E934" s="8"/>
-      <c r="F934" s="8"/>
-      <c r="G934" s="8"/>
-      <c r="H934" s="8"/>
-      <c r="I934" s="8"/>
+      <c r="D934" s="12"/>
+      <c r="E934" s="12"/>
+      <c r="F934" s="12"/>
+      <c r="G934" s="12"/>
+      <c r="H934" s="12"/>
+      <c r="I934" s="12"/>
       <c r="J934" s="2"/>
       <c r="K934" s="2"/>
       <c r="L934" s="2"/>
     </row>
     <row r="935" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D935" s="8"/>
-      <c r="E935" s="8"/>
-      <c r="F935" s="8"/>
-      <c r="G935" s="8"/>
-      <c r="H935" s="8"/>
-      <c r="I935" s="8"/>
+      <c r="D935" s="12"/>
+      <c r="E935" s="12"/>
+      <c r="F935" s="12"/>
+      <c r="G935" s="12"/>
+      <c r="H935" s="12"/>
+      <c r="I935" s="12"/>
       <c r="J935" s="2"/>
       <c r="K935" s="2"/>
       <c r="L935" s="2"/>
@@ -26307,36 +26659,36 @@
       <c r="L952" s="2"/>
     </row>
     <row r="953" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D953" s="8" t="s">
+      <c r="D953" s="12" t="s">
         <v>1023</v>
       </c>
-      <c r="E953" s="8"/>
-      <c r="F953" s="8"/>
-      <c r="G953" s="8"/>
-      <c r="H953" s="8"/>
-      <c r="I953" s="8"/>
+      <c r="E953" s="12"/>
+      <c r="F953" s="12"/>
+      <c r="G953" s="12"/>
+      <c r="H953" s="12"/>
+      <c r="I953" s="12"/>
       <c r="J953" s="2"/>
       <c r="K953" s="2"/>
       <c r="L953" s="2"/>
     </row>
     <row r="954" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D954" s="8"/>
-      <c r="E954" s="8"/>
-      <c r="F954" s="8"/>
-      <c r="G954" s="8"/>
-      <c r="H954" s="8"/>
-      <c r="I954" s="8"/>
+      <c r="D954" s="12"/>
+      <c r="E954" s="12"/>
+      <c r="F954" s="12"/>
+      <c r="G954" s="12"/>
+      <c r="H954" s="12"/>
+      <c r="I954" s="12"/>
       <c r="J954" s="2"/>
       <c r="K954" s="2"/>
       <c r="L954" s="2"/>
     </row>
     <row r="955" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D955" s="8"/>
-      <c r="E955" s="8"/>
-      <c r="F955" s="8"/>
-      <c r="G955" s="8"/>
-      <c r="H955" s="8"/>
-      <c r="I955" s="8"/>
+      <c r="D955" s="12"/>
+      <c r="E955" s="12"/>
+      <c r="F955" s="12"/>
+      <c r="G955" s="12"/>
+      <c r="H955" s="12"/>
+      <c r="I955" s="12"/>
       <c r="J955" s="2"/>
       <c r="K955" s="2"/>
       <c r="L955" s="2"/>
@@ -26628,36 +26980,36 @@
       <c r="L969" s="2"/>
     </row>
     <row r="970" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D970" s="8" t="s">
+      <c r="D970" s="12" t="s">
         <v>1024</v>
       </c>
-      <c r="E970" s="8"/>
-      <c r="F970" s="8"/>
-      <c r="G970" s="8"/>
-      <c r="H970" s="8"/>
-      <c r="I970" s="8"/>
+      <c r="E970" s="12"/>
+      <c r="F970" s="12"/>
+      <c r="G970" s="12"/>
+      <c r="H970" s="12"/>
+      <c r="I970" s="12"/>
       <c r="J970" s="2"/>
       <c r="K970" s="2"/>
       <c r="L970" s="2"/>
     </row>
     <row r="971" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D971" s="8"/>
-      <c r="E971" s="8"/>
-      <c r="F971" s="8"/>
-      <c r="G971" s="8"/>
-      <c r="H971" s="8"/>
-      <c r="I971" s="8"/>
+      <c r="D971" s="12"/>
+      <c r="E971" s="12"/>
+      <c r="F971" s="12"/>
+      <c r="G971" s="12"/>
+      <c r="H971" s="12"/>
+      <c r="I971" s="12"/>
       <c r="J971" s="2"/>
       <c r="K971" s="2"/>
       <c r="L971" s="2"/>
     </row>
     <row r="972" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D972" s="8"/>
-      <c r="E972" s="8"/>
-      <c r="F972" s="8"/>
-      <c r="G972" s="8"/>
-      <c r="H972" s="8"/>
-      <c r="I972" s="8"/>
+      <c r="D972" s="12"/>
+      <c r="E972" s="12"/>
+      <c r="F972" s="12"/>
+      <c r="G972" s="12"/>
+      <c r="H972" s="12"/>
+      <c r="I972" s="12"/>
       <c r="J972" s="2"/>
       <c r="K972" s="2"/>
       <c r="L972" s="2"/>
@@ -27065,10 +27417,10 @@
       <c r="L990" s="2"/>
     </row>
     <row r="991" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A991" s="13">
-        <v>43263</v>
-      </c>
-      <c r="B991" s="14" t="s">
+      <c r="A991" s="10">
+        <v>43263</v>
+      </c>
+      <c r="B991" s="11" t="s">
         <v>747</v>
       </c>
       <c r="C991" s="7" t="s">
@@ -27609,39 +27961,39 @@
       <c r="B1012" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D1012" s="8" t="s">
+      <c r="D1012" s="12" t="s">
         <v>1025</v>
       </c>
-      <c r="E1012" s="8"/>
-      <c r="F1012" s="8"/>
-      <c r="G1012" s="8"/>
-      <c r="H1012" s="8"/>
-      <c r="I1012" s="8"/>
-      <c r="J1012" s="8"/>
-      <c r="K1012" s="8"/>
-      <c r="L1012" s="8"/>
+      <c r="E1012" s="12"/>
+      <c r="F1012" s="12"/>
+      <c r="G1012" s="12"/>
+      <c r="H1012" s="12"/>
+      <c r="I1012" s="12"/>
+      <c r="J1012" s="12"/>
+      <c r="K1012" s="12"/>
+      <c r="L1012" s="12"/>
     </row>
     <row r="1013" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1013" s="8"/>
-      <c r="E1013" s="8"/>
-      <c r="F1013" s="8"/>
-      <c r="G1013" s="8"/>
-      <c r="H1013" s="8"/>
-      <c r="I1013" s="8"/>
-      <c r="J1013" s="8"/>
-      <c r="K1013" s="8"/>
-      <c r="L1013" s="8"/>
+      <c r="D1013" s="12"/>
+      <c r="E1013" s="12"/>
+      <c r="F1013" s="12"/>
+      <c r="G1013" s="12"/>
+      <c r="H1013" s="12"/>
+      <c r="I1013" s="12"/>
+      <c r="J1013" s="12"/>
+      <c r="K1013" s="12"/>
+      <c r="L1013" s="12"/>
     </row>
     <row r="1014" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1014" s="8"/>
-      <c r="E1014" s="8"/>
-      <c r="F1014" s="8"/>
-      <c r="G1014" s="8"/>
-      <c r="H1014" s="8"/>
-      <c r="I1014" s="8"/>
-      <c r="J1014" s="8"/>
-      <c r="K1014" s="8"/>
-      <c r="L1014" s="8"/>
+      <c r="D1014" s="12"/>
+      <c r="E1014" s="12"/>
+      <c r="F1014" s="12"/>
+      <c r="G1014" s="12"/>
+      <c r="H1014" s="12"/>
+      <c r="I1014" s="12"/>
+      <c r="J1014" s="12"/>
+      <c r="K1014" s="12"/>
+      <c r="L1014" s="12"/>
     </row>
     <row r="1015" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1015" s="2"/>
@@ -27960,39 +28312,39 @@
       <c r="B1029" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D1029" s="8" t="s">
+      <c r="D1029" s="12" t="s">
         <v>1026</v>
       </c>
-      <c r="E1029" s="8"/>
-      <c r="F1029" s="8"/>
-      <c r="G1029" s="8"/>
-      <c r="H1029" s="8"/>
-      <c r="I1029" s="8"/>
-      <c r="J1029" s="8"/>
-      <c r="K1029" s="8"/>
-      <c r="L1029" s="8"/>
+      <c r="E1029" s="12"/>
+      <c r="F1029" s="12"/>
+      <c r="G1029" s="12"/>
+      <c r="H1029" s="12"/>
+      <c r="I1029" s="12"/>
+      <c r="J1029" s="12"/>
+      <c r="K1029" s="12"/>
+      <c r="L1029" s="12"/>
     </row>
     <row r="1030" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1030" s="8"/>
-      <c r="E1030" s="8"/>
-      <c r="F1030" s="8"/>
-      <c r="G1030" s="8"/>
-      <c r="H1030" s="8"/>
-      <c r="I1030" s="8"/>
-      <c r="J1030" s="8"/>
-      <c r="K1030" s="8"/>
-      <c r="L1030" s="8"/>
+      <c r="D1030" s="12"/>
+      <c r="E1030" s="12"/>
+      <c r="F1030" s="12"/>
+      <c r="G1030" s="12"/>
+      <c r="H1030" s="12"/>
+      <c r="I1030" s="12"/>
+      <c r="J1030" s="12"/>
+      <c r="K1030" s="12"/>
+      <c r="L1030" s="12"/>
     </row>
     <row r="1031" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1031" s="8"/>
-      <c r="E1031" s="8"/>
-      <c r="F1031" s="8"/>
-      <c r="G1031" s="8"/>
-      <c r="H1031" s="8"/>
-      <c r="I1031" s="8"/>
-      <c r="J1031" s="8"/>
-      <c r="K1031" s="8"/>
-      <c r="L1031" s="8"/>
+      <c r="D1031" s="12"/>
+      <c r="E1031" s="12"/>
+      <c r="F1031" s="12"/>
+      <c r="G1031" s="12"/>
+      <c r="H1031" s="12"/>
+      <c r="I1031" s="12"/>
+      <c r="J1031" s="12"/>
+      <c r="K1031" s="12"/>
+      <c r="L1031" s="12"/>
     </row>
     <row r="1032" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1032" s="2"/>
@@ -29298,36 +29650,36 @@
       <c r="L1081" s="2"/>
     </row>
     <row r="1082" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1082" s="8" t="s">
+      <c r="D1082" s="12" t="s">
         <v>1027</v>
       </c>
-      <c r="E1082" s="8"/>
-      <c r="F1082" s="8"/>
-      <c r="G1082" s="8"/>
-      <c r="H1082" s="8"/>
-      <c r="I1082" s="8"/>
+      <c r="E1082" s="12"/>
+      <c r="F1082" s="12"/>
+      <c r="G1082" s="12"/>
+      <c r="H1082" s="12"/>
+      <c r="I1082" s="12"/>
       <c r="J1082" s="2"/>
       <c r="K1082" s="2"/>
       <c r="L1082" s="2"/>
     </row>
     <row r="1083" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1083" s="8"/>
-      <c r="E1083" s="8"/>
-      <c r="F1083" s="8"/>
-      <c r="G1083" s="8"/>
-      <c r="H1083" s="8"/>
-      <c r="I1083" s="8"/>
+      <c r="D1083" s="12"/>
+      <c r="E1083" s="12"/>
+      <c r="F1083" s="12"/>
+      <c r="G1083" s="12"/>
+      <c r="H1083" s="12"/>
+      <c r="I1083" s="12"/>
       <c r="J1083" s="2"/>
       <c r="K1083" s="2"/>
       <c r="L1083" s="2"/>
     </row>
     <row r="1084" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1084" s="8"/>
-      <c r="E1084" s="8"/>
-      <c r="F1084" s="8"/>
-      <c r="G1084" s="8"/>
-      <c r="H1084" s="8"/>
-      <c r="I1084" s="8"/>
+      <c r="D1084" s="12"/>
+      <c r="E1084" s="12"/>
+      <c r="F1084" s="12"/>
+      <c r="G1084" s="12"/>
+      <c r="H1084" s="12"/>
+      <c r="I1084" s="12"/>
       <c r="J1084" s="2"/>
       <c r="K1084" s="2"/>
       <c r="L1084" s="2"/>
@@ -30901,39 +31253,39 @@
       <c r="B1141" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D1141" s="8" t="s">
+      <c r="D1141" s="12" t="s">
         <v>1028</v>
       </c>
-      <c r="E1141" s="8"/>
-      <c r="F1141" s="8"/>
-      <c r="G1141" s="8"/>
-      <c r="H1141" s="8"/>
-      <c r="I1141" s="8"/>
-      <c r="J1141" s="8"/>
-      <c r="K1141" s="8"/>
-      <c r="L1141" s="8"/>
+      <c r="E1141" s="12"/>
+      <c r="F1141" s="12"/>
+      <c r="G1141" s="12"/>
+      <c r="H1141" s="12"/>
+      <c r="I1141" s="12"/>
+      <c r="J1141" s="12"/>
+      <c r="K1141" s="12"/>
+      <c r="L1141" s="12"/>
     </row>
     <row r="1142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1142" s="8"/>
-      <c r="E1142" s="8"/>
-      <c r="F1142" s="8"/>
-      <c r="G1142" s="8"/>
-      <c r="H1142" s="8"/>
-      <c r="I1142" s="8"/>
-      <c r="J1142" s="8"/>
-      <c r="K1142" s="8"/>
-      <c r="L1142" s="8"/>
+      <c r="D1142" s="12"/>
+      <c r="E1142" s="12"/>
+      <c r="F1142" s="12"/>
+      <c r="G1142" s="12"/>
+      <c r="H1142" s="12"/>
+      <c r="I1142" s="12"/>
+      <c r="J1142" s="12"/>
+      <c r="K1142" s="12"/>
+      <c r="L1142" s="12"/>
     </row>
     <row r="1143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1143" s="8"/>
-      <c r="E1143" s="8"/>
-      <c r="F1143" s="8"/>
-      <c r="G1143" s="8"/>
-      <c r="H1143" s="8"/>
-      <c r="I1143" s="8"/>
-      <c r="J1143" s="8"/>
-      <c r="K1143" s="8"/>
-      <c r="L1143" s="8"/>
+      <c r="D1143" s="12"/>
+      <c r="E1143" s="12"/>
+      <c r="F1143" s="12"/>
+      <c r="G1143" s="12"/>
+      <c r="H1143" s="12"/>
+      <c r="I1143" s="12"/>
+      <c r="J1143" s="12"/>
+      <c r="K1143" s="12"/>
+      <c r="L1143" s="12"/>
     </row>
     <row r="1144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1144" s="2"/>
@@ -32142,39 +32494,39 @@
       <c r="B1189" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D1189" s="8" t="s">
+      <c r="D1189" s="12" t="s">
         <v>1029</v>
       </c>
-      <c r="E1189" s="8"/>
-      <c r="F1189" s="8"/>
-      <c r="G1189" s="8"/>
-      <c r="H1189" s="8"/>
-      <c r="I1189" s="8"/>
-      <c r="J1189" s="8"/>
-      <c r="K1189" s="8"/>
-      <c r="L1189" s="8"/>
+      <c r="E1189" s="12"/>
+      <c r="F1189" s="12"/>
+      <c r="G1189" s="12"/>
+      <c r="H1189" s="12"/>
+      <c r="I1189" s="12"/>
+      <c r="J1189" s="12"/>
+      <c r="K1189" s="12"/>
+      <c r="L1189" s="12"/>
     </row>
     <row r="1190" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1190" s="8"/>
-      <c r="E1190" s="8"/>
-      <c r="F1190" s="8"/>
-      <c r="G1190" s="8"/>
-      <c r="H1190" s="8"/>
-      <c r="I1190" s="8"/>
-      <c r="J1190" s="8"/>
-      <c r="K1190" s="8"/>
-      <c r="L1190" s="8"/>
+      <c r="D1190" s="12"/>
+      <c r="E1190" s="12"/>
+      <c r="F1190" s="12"/>
+      <c r="G1190" s="12"/>
+      <c r="H1190" s="12"/>
+      <c r="I1190" s="12"/>
+      <c r="J1190" s="12"/>
+      <c r="K1190" s="12"/>
+      <c r="L1190" s="12"/>
     </row>
     <row r="1191" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D1191" s="8"/>
-      <c r="E1191" s="8"/>
-      <c r="F1191" s="8"/>
-      <c r="G1191" s="8"/>
-      <c r="H1191" s="8"/>
-      <c r="I1191" s="8"/>
-      <c r="J1191" s="8"/>
-      <c r="K1191" s="8"/>
-      <c r="L1191" s="8"/>
+      <c r="D1191" s="12"/>
+      <c r="E1191" s="12"/>
+      <c r="F1191" s="12"/>
+      <c r="G1191" s="12"/>
+      <c r="H1191" s="12"/>
+      <c r="I1191" s="12"/>
+      <c r="J1191" s="12"/>
+      <c r="K1191" s="12"/>
+      <c r="L1191" s="12"/>
     </row>
     <row r="1192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1192" s="2"/>
@@ -32189,15 +32541,16 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="D495:L497"/>
-    <mergeCell ref="D849:L851"/>
-    <mergeCell ref="D866:L868"/>
-    <mergeCell ref="D883:L885"/>
-    <mergeCell ref="D1012:L1014"/>
-    <mergeCell ref="D912:I914"/>
-    <mergeCell ref="D933:I935"/>
-    <mergeCell ref="D953:I955"/>
-    <mergeCell ref="D970:I972"/>
+    <mergeCell ref="D9:L11"/>
+    <mergeCell ref="D50:L52"/>
+    <mergeCell ref="D95:L97"/>
+    <mergeCell ref="D309:L311"/>
+    <mergeCell ref="D561:I563"/>
+    <mergeCell ref="D476:I478"/>
+    <mergeCell ref="D423:I425"/>
+    <mergeCell ref="D440:I442"/>
+    <mergeCell ref="D459:I461"/>
+    <mergeCell ref="D522:I524"/>
     <mergeCell ref="D1029:L1031"/>
     <mergeCell ref="D1141:L1143"/>
     <mergeCell ref="D1189:L1191"/>
@@ -32208,22 +32561,21 @@
     <mergeCell ref="D218:I220"/>
     <mergeCell ref="D269:I271"/>
     <mergeCell ref="D292:I294"/>
-    <mergeCell ref="D9:L11"/>
-    <mergeCell ref="D50:L52"/>
-    <mergeCell ref="D95:L97"/>
-    <mergeCell ref="D309:L311"/>
-    <mergeCell ref="D561:I563"/>
     <mergeCell ref="D1082:I1084"/>
-    <mergeCell ref="D476:I478"/>
     <mergeCell ref="D571:I573"/>
-    <mergeCell ref="D423:I425"/>
-    <mergeCell ref="D440:I442"/>
-    <mergeCell ref="D459:I461"/>
-    <mergeCell ref="D522:I524"/>
     <mergeCell ref="D587:I589"/>
     <mergeCell ref="D606:I608"/>
     <mergeCell ref="D623:I625"/>
     <mergeCell ref="D651:I653"/>
+    <mergeCell ref="D495:L497"/>
+    <mergeCell ref="D849:L851"/>
+    <mergeCell ref="D866:L868"/>
+    <mergeCell ref="D883:L885"/>
+    <mergeCell ref="D1012:L1014"/>
+    <mergeCell ref="D912:I914"/>
+    <mergeCell ref="D933:I935"/>
+    <mergeCell ref="D953:I955"/>
+    <mergeCell ref="D970:I972"/>
     <mergeCell ref="D789:I791"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32236,19 +32588,537 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
-      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
-      <Description>STHNKY6CXN64-585-23125</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>6</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023C68C9F20C69D48BB417A9ADFD5DC9C" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29914a5778ec744f9d5d623c4355d354">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03a57c4080a7a73066863a39e6ec4255" ns2:_="">
     <xsd:import namespace="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
@@ -32393,7 +33263,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
+      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
+      <Description>STHNKY6CXN64-585-23125</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -32439,26 +33330,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02EC59C-3037-4324-9F25-70F5C5DE4AE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4983C0FC-0A52-42BE-81C3-B1D565BD5AB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32476,18 +33348,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02EC59C-3037-4324-9F25-70F5C5DE4AE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730136FF-7953-4B5D-A700-45AC58366C1D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDFF90A1-0238-4E08-AF86-38ADE0A38CA8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730136FF-7953-4B5D-A700-45AC58366C1D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
James Martinez - New Modifications, updates to Service indicators and test scores for 20180702 Data Federation meeting. Publishing to data.ufl.edu. Updated with Crosswalk tab
</commit_message>
<xml_diff>
--- a/Reporting_Student_Data_Model_Dictionary.xlsx
+++ b/Reporting_Student_Data_Model_Dictionary.xlsx
@@ -9096,9 +9096,7 @@
 </file>
 
 <file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{74F0CE91-FC60-44BC-8FE0-2AEF68936F4B}" name="Martinez,James J" id="-584524543" dateTime="2018-06-27T17:14:41"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
James Martinez - 8/29 updates: WH_STUDENT_STATUS_TERM columns part 3
</commit_message>
<xml_diff>
--- a/Reporting_Student_Data_Model_Dictionary.xlsx
+++ b/Reporting_Student_Data_Model_Dictionary.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7151" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7155" uniqueCount="1765">
   <si>
     <t>Owner</t>
   </si>
@@ -6297,6 +6297,15 @@
   </si>
   <si>
     <t>A grade point deficit is defined as the number of grade points below a C average on credits attempted at UF. If the grade point average is less than 2.0, there is a grade point deficit. Only grades higher than C (2.0) will lower a deficit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIVERSAL_TRACKING_TERM_CD </t>
+  </si>
+  <si>
+    <t>UF_UNIV_TRK_TER</t>
+  </si>
+  <si>
+    <t>Universal Tracking Semester Code</t>
   </si>
 </sst>
 </file>
@@ -6432,10 +6441,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11625,7 +11634,7 @@
       <c r="B199" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D199" s="23" t="s">
+      <c r="D199" s="24" t="s">
         <v>992</v>
       </c>
       <c r="E199" s="22"/>
@@ -12691,7 +12700,7 @@
       <c r="B244" s="6" t="s">
         <v>722</v>
       </c>
-      <c r="D244" s="23" t="s">
+      <c r="D244" s="24" t="s">
         <v>991</v>
       </c>
       <c r="E244" s="22"/>
@@ -14396,36 +14405,36 @@
       <c r="L317" s="2"/>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D318" s="24" t="s">
+      <c r="D318" s="23" t="s">
         <v>999</v>
       </c>
-      <c r="E318" s="24"/>
-      <c r="F318" s="24"/>
-      <c r="G318" s="24"/>
-      <c r="H318" s="24"/>
-      <c r="I318" s="24"/>
+      <c r="E318" s="23"/>
+      <c r="F318" s="23"/>
+      <c r="G318" s="23"/>
+      <c r="H318" s="23"/>
+      <c r="I318" s="23"/>
       <c r="J318" s="2"/>
       <c r="K318" s="2"/>
       <c r="L318" s="2"/>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D319" s="24"/>
-      <c r="E319" s="24"/>
-      <c r="F319" s="24"/>
-      <c r="G319" s="24"/>
-      <c r="H319" s="24"/>
-      <c r="I319" s="24"/>
+      <c r="D319" s="23"/>
+      <c r="E319" s="23"/>
+      <c r="F319" s="23"/>
+      <c r="G319" s="23"/>
+      <c r="H319" s="23"/>
+      <c r="I319" s="23"/>
       <c r="J319" s="2"/>
       <c r="K319" s="2"/>
       <c r="L319" s="2"/>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D320" s="24"/>
-      <c r="E320" s="24"/>
-      <c r="F320" s="24"/>
-      <c r="G320" s="24"/>
-      <c r="H320" s="24"/>
-      <c r="I320" s="24"/>
+      <c r="D320" s="23"/>
+      <c r="E320" s="23"/>
+      <c r="F320" s="23"/>
+      <c r="G320" s="23"/>
+      <c r="H320" s="23"/>
+      <c r="I320" s="23"/>
       <c r="J320" s="2"/>
       <c r="K320" s="2"/>
       <c r="L320" s="2"/>
@@ -15380,36 +15389,36 @@
       <c r="L362" s="2"/>
     </row>
     <row r="363" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D363" s="24" t="s">
+      <c r="D363" s="23" t="s">
         <v>1001</v>
       </c>
-      <c r="E363" s="24"/>
-      <c r="F363" s="24"/>
-      <c r="G363" s="24"/>
-      <c r="H363" s="24"/>
-      <c r="I363" s="24"/>
+      <c r="E363" s="23"/>
+      <c r="F363" s="23"/>
+      <c r="G363" s="23"/>
+      <c r="H363" s="23"/>
+      <c r="I363" s="23"/>
       <c r="J363" s="2"/>
       <c r="K363" s="2"/>
       <c r="L363" s="2"/>
     </row>
     <row r="364" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D364" s="24"/>
-      <c r="E364" s="24"/>
-      <c r="F364" s="24"/>
-      <c r="G364" s="24"/>
-      <c r="H364" s="24"/>
-      <c r="I364" s="24"/>
+      <c r="D364" s="23"/>
+      <c r="E364" s="23"/>
+      <c r="F364" s="23"/>
+      <c r="G364" s="23"/>
+      <c r="H364" s="23"/>
+      <c r="I364" s="23"/>
       <c r="J364" s="2"/>
       <c r="K364" s="2"/>
       <c r="L364" s="2"/>
     </row>
     <row r="365" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D365" s="24"/>
-      <c r="E365" s="24"/>
-      <c r="F365" s="24"/>
-      <c r="G365" s="24"/>
-      <c r="H365" s="24"/>
-      <c r="I365" s="24"/>
+      <c r="D365" s="23"/>
+      <c r="E365" s="23"/>
+      <c r="F365" s="23"/>
+      <c r="G365" s="23"/>
+      <c r="H365" s="23"/>
+      <c r="I365" s="23"/>
       <c r="J365" s="2"/>
       <c r="K365" s="2"/>
       <c r="L365" s="2"/>
@@ -17406,36 +17415,36 @@
       <c r="L448" s="2"/>
     </row>
     <row r="449" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D449" s="24" t="s">
+      <c r="D449" s="23" t="s">
         <v>1002</v>
       </c>
-      <c r="E449" s="24"/>
-      <c r="F449" s="24"/>
-      <c r="G449" s="24"/>
-      <c r="H449" s="24"/>
-      <c r="I449" s="24"/>
+      <c r="E449" s="23"/>
+      <c r="F449" s="23"/>
+      <c r="G449" s="23"/>
+      <c r="H449" s="23"/>
+      <c r="I449" s="23"/>
       <c r="J449" s="2"/>
       <c r="K449" s="2"/>
       <c r="L449" s="2"/>
     </row>
     <row r="450" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D450" s="24"/>
-      <c r="E450" s="24"/>
-      <c r="F450" s="24"/>
-      <c r="G450" s="24"/>
-      <c r="H450" s="24"/>
-      <c r="I450" s="24"/>
+      <c r="D450" s="23"/>
+      <c r="E450" s="23"/>
+      <c r="F450" s="23"/>
+      <c r="G450" s="23"/>
+      <c r="H450" s="23"/>
+      <c r="I450" s="23"/>
       <c r="J450" s="2"/>
       <c r="K450" s="2"/>
       <c r="L450" s="2"/>
     </row>
     <row r="451" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D451" s="24"/>
-      <c r="E451" s="24"/>
-      <c r="F451" s="24"/>
-      <c r="G451" s="24"/>
-      <c r="H451" s="24"/>
-      <c r="I451" s="24"/>
+      <c r="D451" s="23"/>
+      <c r="E451" s="23"/>
+      <c r="F451" s="23"/>
+      <c r="G451" s="23"/>
+      <c r="H451" s="23"/>
+      <c r="I451" s="23"/>
       <c r="J451" s="2"/>
       <c r="K451" s="2"/>
       <c r="L451" s="2"/>
@@ -36447,7 +36456,7 @@
       <c r="B1252" s="6" t="s">
         <v>1163</v>
       </c>
-      <c r="D1252" s="23" t="s">
+      <c r="D1252" s="24" t="s">
         <v>1287</v>
       </c>
       <c r="E1252" s="22"/>
@@ -41122,38 +41131,38 @@
     </row>
     <row r="1468" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1468" s="4"/>
-      <c r="D1468" s="23" t="s">
+      <c r="D1468" s="24" t="s">
         <v>1653</v>
       </c>
-      <c r="E1468" s="23"/>
-      <c r="F1468" s="23"/>
-      <c r="G1468" s="23"/>
-      <c r="H1468" s="23"/>
-      <c r="I1468" s="23"/>
+      <c r="E1468" s="24"/>
+      <c r="F1468" s="24"/>
+      <c r="G1468" s="24"/>
+      <c r="H1468" s="24"/>
+      <c r="I1468" s="24"/>
       <c r="J1468" s="17"/>
       <c r="K1468" s="17"/>
       <c r="L1468" s="17"/>
     </row>
     <row r="1469" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1469" s="4"/>
-      <c r="D1469" s="23"/>
-      <c r="E1469" s="23"/>
-      <c r="F1469" s="23"/>
-      <c r="G1469" s="23"/>
-      <c r="H1469" s="23"/>
-      <c r="I1469" s="23"/>
+      <c r="D1469" s="24"/>
+      <c r="E1469" s="24"/>
+      <c r="F1469" s="24"/>
+      <c r="G1469" s="24"/>
+      <c r="H1469" s="24"/>
+      <c r="I1469" s="24"/>
       <c r="J1469" s="17"/>
       <c r="K1469" s="17"/>
       <c r="L1469" s="17"/>
     </row>
     <row r="1470" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1470" s="4"/>
-      <c r="D1470" s="23"/>
-      <c r="E1470" s="23"/>
-      <c r="F1470" s="23"/>
-      <c r="G1470" s="23"/>
-      <c r="H1470" s="23"/>
-      <c r="I1470" s="23"/>
+      <c r="D1470" s="24"/>
+      <c r="E1470" s="24"/>
+      <c r="F1470" s="24"/>
+      <c r="G1470" s="24"/>
+      <c r="H1470" s="24"/>
+      <c r="I1470" s="24"/>
       <c r="J1470" s="17"/>
       <c r="K1470" s="17"/>
       <c r="L1470" s="17"/>
@@ -42361,7 +42370,7 @@
       </c>
     </row>
     <row r="1522" spans="4:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1522" s="23" t="s">
+      <c r="D1522" s="24" t="s">
         <v>1654</v>
       </c>
       <c r="E1522" s="22"/>
@@ -42405,29 +42414,7 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="49">
-    <mergeCell ref="D1236:L1238"/>
-    <mergeCell ref="D1129:I1131"/>
-    <mergeCell ref="D295:I297"/>
-    <mergeCell ref="D318:I320"/>
-    <mergeCell ref="D1468:I1470"/>
-    <mergeCell ref="D1484:I1486"/>
-    <mergeCell ref="D1522:I1524"/>
-    <mergeCell ref="D835:I837"/>
-    <mergeCell ref="D895:L897"/>
-    <mergeCell ref="D912:L914"/>
-    <mergeCell ref="D929:L931"/>
-    <mergeCell ref="D1059:L1061"/>
-    <mergeCell ref="D958:I960"/>
-    <mergeCell ref="D979:I981"/>
-    <mergeCell ref="D999:I1001"/>
-    <mergeCell ref="D1016:I1018"/>
-    <mergeCell ref="D1076:L1078"/>
-    <mergeCell ref="D1188:L1190"/>
-    <mergeCell ref="D613:I615"/>
-    <mergeCell ref="D629:I631"/>
-    <mergeCell ref="D648:I650"/>
-    <mergeCell ref="D665:I667"/>
-    <mergeCell ref="D693:I695"/>
+    <mergeCell ref="D1421:L1423"/>
     <mergeCell ref="D17:L19"/>
     <mergeCell ref="D68:L70"/>
     <mergeCell ref="D113:L115"/>
@@ -42444,16 +42431,38 @@
     <mergeCell ref="D143:I145"/>
     <mergeCell ref="D199:I201"/>
     <mergeCell ref="D244:I246"/>
+    <mergeCell ref="D1484:I1486"/>
+    <mergeCell ref="D1522:I1524"/>
+    <mergeCell ref="D835:I837"/>
+    <mergeCell ref="D895:L897"/>
+    <mergeCell ref="D912:L914"/>
+    <mergeCell ref="D929:L931"/>
+    <mergeCell ref="D1059:L1061"/>
+    <mergeCell ref="D958:I960"/>
+    <mergeCell ref="D979:I981"/>
+    <mergeCell ref="D999:I1001"/>
+    <mergeCell ref="D1016:I1018"/>
+    <mergeCell ref="D1076:L1078"/>
+    <mergeCell ref="D1188:L1190"/>
     <mergeCell ref="D1252:L1254"/>
     <mergeCell ref="D1267:L1269"/>
     <mergeCell ref="D1292:L1294"/>
+    <mergeCell ref="D1236:L1238"/>
+    <mergeCell ref="D1129:I1131"/>
+    <mergeCell ref="D295:I297"/>
+    <mergeCell ref="D318:I320"/>
+    <mergeCell ref="D1468:I1470"/>
+    <mergeCell ref="D613:I615"/>
+    <mergeCell ref="D629:I631"/>
+    <mergeCell ref="D648:I650"/>
+    <mergeCell ref="D665:I667"/>
+    <mergeCell ref="D693:I695"/>
     <mergeCell ref="D1309:L1311"/>
     <mergeCell ref="D1326:L1328"/>
     <mergeCell ref="D1431:L1433"/>
     <mergeCell ref="D1346:L1348"/>
     <mergeCell ref="D1361:L1363"/>
     <mergeCell ref="D1386:L1388"/>
-    <mergeCell ref="D1421:L1423"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -43287,10 +43296,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44113,15 +44122,15 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>1436</v>
+        <v>1763</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>1718</v>
+        <v>1762</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>1527</v>
+        <v>1764</v>
       </c>
       <c r="D59" s="21" t="s">
         <v>1574</v>
@@ -44129,13 +44138,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D60" s="21" t="s">
         <v>1574</v>
@@ -44143,13 +44152,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="21" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D61" s="21" t="s">
         <v>1574</v>
@@ -44157,13 +44166,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="21" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>1303</v>
+        <v>1720</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>1574</v>
@@ -44171,13 +44180,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="21" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>1721</v>
+        <v>1303</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="D63" s="21" t="s">
         <v>1574</v>
@@ -44185,41 +44194,41 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="21" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>1531</v>
+        <v>1533</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>1532</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>1574</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="D66" s="21" t="s">
         <v>1574</v>
@@ -44227,13 +44236,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>1574</v>
@@ -44241,13 +44250,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="D68" s="21" t="s">
         <v>1574</v>
@@ -44255,13 +44264,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D69" s="21" t="s">
         <v>1574</v>
@@ -44269,13 +44278,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="D70" s="21" t="s">
         <v>1574</v>
@@ -44283,13 +44292,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D71" s="21" t="s">
         <v>1574</v>
@@ -44297,13 +44306,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="D72" s="21" t="s">
         <v>1574</v>
@@ -44311,13 +44320,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="D73" s="21" t="s">
         <v>1574</v>
@@ -44325,13 +44334,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="D74" s="21" t="s">
         <v>1574</v>
@@ -44339,13 +44348,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>1574</v>
@@ -44353,13 +44362,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="D76" s="21" t="s">
         <v>1574</v>
@@ -44367,13 +44376,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="21" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D77" s="21" t="s">
         <v>1574</v>
@@ -44381,13 +44390,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>1564</v>
+        <v>1546</v>
       </c>
       <c r="D78" s="21" t="s">
         <v>1574</v>
@@ -44395,13 +44404,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>1562</v>
+        <v>1564</v>
       </c>
       <c r="D79" s="21" t="s">
         <v>1574</v>
@@ -44409,13 +44418,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="D80" s="21" t="s">
         <v>1574</v>
@@ -44423,13 +44432,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>1561</v>
+        <v>1563</v>
       </c>
       <c r="D81" s="21" t="s">
         <v>1574</v>
@@ -44437,13 +44446,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="21" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="D82" s="21" t="s">
         <v>1574</v>
@@ -44451,13 +44460,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="21" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="D83" s="21" t="s">
         <v>1574</v>
@@ -44465,13 +44474,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="21" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="D84" s="21" t="s">
         <v>1574</v>
@@ -44479,13 +44488,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="21" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="D85" s="21" t="s">
         <v>1574</v>
@@ -44493,13 +44502,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="21" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="D86" s="21" t="s">
         <v>1574</v>
@@ -44507,13 +44516,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>1554</v>
+        <v>1556</v>
       </c>
       <c r="D87" s="21" t="s">
         <v>1574</v>
@@ -44521,13 +44530,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="D88" s="21" t="s">
         <v>1574</v>
@@ -44535,13 +44544,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>1553</v>
+        <v>1555</v>
       </c>
       <c r="D89" s="21" t="s">
         <v>1574</v>
@@ -44549,13 +44558,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>1547</v>
+        <v>1553</v>
       </c>
       <c r="D90" s="21" t="s">
         <v>1574</v>
@@ -44563,13 +44572,13 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="21" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="D91" s="21" t="s">
         <v>1574</v>
@@ -44577,13 +44586,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="D92" s="21" t="s">
         <v>1574</v>
@@ -44591,13 +44600,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="21" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="D93" s="21" t="s">
         <v>1574</v>
@@ -44605,13 +44614,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="D94" s="21" t="s">
         <v>1574</v>
@@ -44619,13 +44628,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="D95" s="21" t="s">
         <v>1574</v>
@@ -44633,27 +44642,27 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>1565</v>
+        <v>1551</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>1755</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="D97" s="21" t="s">
         <v>1755</v>
@@ -44661,13 +44670,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D98" s="21" t="s">
         <v>1755</v>
@@ -44675,13 +44684,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="21" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D99" s="21" t="s">
         <v>1755</v>
@@ -44689,27 +44698,27 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="21" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>686</v>
+        <v>1758</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>1574</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="21" t="s">
-        <v>1664</v>
+        <v>1477</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>1759</v>
+        <v>686</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>1665</v>
+        <v>1569</v>
       </c>
       <c r="D101" s="21" t="s">
         <v>1574</v>
@@ -44717,13 +44726,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="21" t="s">
-        <v>820</v>
+        <v>1664</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>820</v>
+        <v>1759</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>1572</v>
+        <v>1665</v>
       </c>
       <c r="D102" s="21" t="s">
         <v>1574</v>
@@ -44731,13 +44740,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="21" t="s">
-        <v>720</v>
+        <v>820</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>720</v>
+        <v>820</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>1570</v>
+        <v>1572</v>
       </c>
       <c r="D103" s="21" t="s">
         <v>1574</v>
@@ -44745,13 +44754,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
-        <v>1478</v>
+        <v>720</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>1478</v>
+        <v>720</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D104" s="21" t="s">
         <v>1574</v>
@@ -44759,13 +44768,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="21" t="s">
-        <v>1365</v>
+        <v>1478</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>1365</v>
+        <v>1478</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="D105" s="21" t="s">
         <v>1574</v>
@@ -44773,29 +44782,43 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="21" t="s">
-        <v>63</v>
+        <v>1365</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>63</v>
+        <v>1365</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>64</v>
+        <v>1573</v>
       </c>
       <c r="D106" s="21" t="s">
         <v>1574</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="19" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D107" s="21" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="19" t="s">
         <v>1686</v>
       </c>
-      <c r="B107" s="21" t="s">
+      <c r="B108" s="21" t="s">
         <v>1760</v>
       </c>
-      <c r="C107" s="18" t="s">
+      <c r="C108" s="18" t="s">
         <v>1761</v>
       </c>
-      <c r="D107" s="21" t="s">
+      <c r="D108" s="21" t="s">
         <v>1574</v>
       </c>
     </row>
@@ -44813,27 +44836,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
-      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
-      <Description>STHNKY6CXN64-585-23125</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010023C68C9F20C69D48BB417A9ADFD5DC9C" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29914a5778ec744f9d5d623c4355d354">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03a57c4080a7a73066863a39e6ec4255" ns2:_="">
     <xsd:import namespace="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
@@ -44978,6 +44980,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
+      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
+      <Description>STHNKY6CXN64-585-23125</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -45025,9 +45048,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730136FF-7953-4B5D-A700-45AC58366C1D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4983C0FC-0A52-42BE-81C3-B1D565BD5AB0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45049,19 +45082,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4983C0FC-0A52-42BE-81C3-B1D565BD5AB0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{730136FF-7953-4B5D-A700-45AC58366C1D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
James Martinez - 9/25 Updated: WH_F_MILESTONES
</commit_message>
<xml_diff>
--- a/Reporting_Student_Data_Model_Dictionary.xlsx
+++ b/Reporting_Student_Data_Model_Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="10365" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24960" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8523" uniqueCount="1977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8668" uniqueCount="2003">
   <si>
     <t>Owner</t>
   </si>
@@ -6944,6 +6944,96 @@
   </si>
   <si>
     <t>WH_STU_APP_INFO_MERGE</t>
+  </si>
+  <si>
+    <t>WH_F_MILESTONES</t>
+  </si>
+  <si>
+    <t>MILESTONE_NUM</t>
+  </si>
+  <si>
+    <t>MILESTONE_CD</t>
+  </si>
+  <si>
+    <t>MILESTONE_LD</t>
+  </si>
+  <si>
+    <t>MILESTONE_FD</t>
+  </si>
+  <si>
+    <t>MILESTONE_LEVEL_CD</t>
+  </si>
+  <si>
+    <t>MILESTONE_LEVEL_LD</t>
+  </si>
+  <si>
+    <t>MILESTONE_TITLE</t>
+  </si>
+  <si>
+    <t>TERM_REQ</t>
+  </si>
+  <si>
+    <t>TERM_REQ_SID</t>
+  </si>
+  <si>
+    <t>ATTEMPT_NUM</t>
+  </si>
+  <si>
+    <t>DT_ATTEMPTED</t>
+  </si>
+  <si>
+    <t>Milestone Number</t>
+  </si>
+  <si>
+    <t>Milestone Code</t>
+  </si>
+  <si>
+    <t>Milestone Long Description</t>
+  </si>
+  <si>
+    <t>Milestone Formal Description</t>
+  </si>
+  <si>
+    <t>Milestone Level Code</t>
+  </si>
+  <si>
+    <t>Milestone Level Long Description</t>
+  </si>
+  <si>
+    <t>Milestone Title</t>
+  </si>
+  <si>
+    <t>Required Term (for Milestone)</t>
+  </si>
+  <si>
+    <t>Required Term Surrogate identification</t>
+  </si>
+  <si>
+    <t>Milestone Attempt Number</t>
+  </si>
+  <si>
+    <t>Flag Indicating if the Milestone is complete</t>
+  </si>
+  <si>
+    <t>Milestone Attempt Date</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Description: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WH_F_MILESTONES  is a fact table that contains the measures of the milestones information.  Milestones are non-course-related events that a student must fulfill for a degree. They include things such as language requirements, qualifying and oral examinations, thesis, and dissertation. Surrogate identifiers should be used to joined to dimensions based on how you want to describe the data.</t>
+    </r>
+  </si>
+  <si>
+    <t>MILESTONE_COMPLETE_FLAG</t>
   </si>
 </sst>
 </file>
@@ -7399,12 +7489,12 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:L1524"/>
+  <dimension ref="A1:L1554"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1491" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1522" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B1352" sqref="B1352"/>
+      <selection pane="bottomLeft" activeCell="I1543" sqref="I1543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43010,7 +43100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="1522" spans="4:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1522" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1522" s="23" t="s">
         <v>1653</v>
       </c>
@@ -43023,7 +43113,7 @@
       <c r="K1522" s="17"/>
       <c r="L1522" s="17"/>
     </row>
-    <row r="1523" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="1523" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1523" s="24"/>
       <c r="E1523" s="24"/>
       <c r="F1523" s="24"/>
@@ -43034,7 +43124,7 @@
       <c r="K1523" s="17"/>
       <c r="L1523" s="17"/>
     </row>
-    <row r="1524" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="1524" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1524" s="24"/>
       <c r="E1524" s="24"/>
       <c r="F1524" s="24"/>
@@ -43045,6 +43135,700 @@
       <c r="K1524" s="17"/>
       <c r="L1524" s="17"/>
     </row>
+    <row r="1527" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1527" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1527" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1527" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1527" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1527" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1527" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1527" s="19">
+        <v>11</v>
+      </c>
+      <c r="H1527" s="19"/>
+      <c r="I1527" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1528" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1528" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1528" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1528" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1528" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1528" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1528" s="19">
+        <v>4</v>
+      </c>
+      <c r="H1528" s="19"/>
+      <c r="I1528" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1529" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1529" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1529" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1529" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1529" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1529" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1529" s="19">
+        <v>5</v>
+      </c>
+      <c r="H1529" s="19"/>
+      <c r="I1529" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1530" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1530" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1530" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1530" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1530" s="19" t="s">
+        <v>679</v>
+      </c>
+      <c r="F1530" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1530" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1530" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1530" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1531" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1531" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1531" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1531" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1531" s="19" t="s">
+        <v>680</v>
+      </c>
+      <c r="F1531" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1531" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1531" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1531" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1532" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1532" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1532" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1532" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1532" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1532" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1532" s="19">
+        <v>10</v>
+      </c>
+      <c r="H1532" s="19"/>
+      <c r="I1532" s="21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1533" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1533" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1533" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1533" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1533" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1533" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1533" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1533" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1533" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1534" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1534" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1534" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1534" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1534" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1534" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1534" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1534" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1534" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1535" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1535" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1535" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1535" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1535" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1535" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1535" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1535" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1535" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1536" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1536" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1536" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1536" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1536" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1536" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1536" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1536" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1536" s="19" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1537" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1537" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1537" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1537" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1537" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1537" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1537" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1537" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1537" s="19" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1538" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1538" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1538" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1538" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1538" s="19" t="s">
+        <v>1978</v>
+      </c>
+      <c r="F1538" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1538" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1538" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1538" t="s">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1539" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1539" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1539" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1539" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1539" s="19" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F1539" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1539" s="19">
+        <v>10</v>
+      </c>
+      <c r="H1539" s="19"/>
+      <c r="I1539" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1540" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1540" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1540" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1540" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1540" s="19" t="s">
+        <v>1980</v>
+      </c>
+      <c r="F1540" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1540" s="19">
+        <v>30</v>
+      </c>
+      <c r="H1540" s="19"/>
+      <c r="I1540" t="s">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1541" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1541" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1541" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1541" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1541" s="19" t="s">
+        <v>1981</v>
+      </c>
+      <c r="F1541" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1541" s="19">
+        <v>50</v>
+      </c>
+      <c r="H1541" s="19"/>
+      <c r="I1541" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1542" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1542" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1542" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1542" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1542" s="19" t="s">
+        <v>1982</v>
+      </c>
+      <c r="F1542" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1542" s="19">
+        <v>15</v>
+      </c>
+      <c r="H1542" s="19"/>
+      <c r="I1542" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1543" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1543" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1543" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1543" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1543" s="19" t="s">
+        <v>1983</v>
+      </c>
+      <c r="F1543" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1543" s="19">
+        <v>30</v>
+      </c>
+      <c r="H1543" s="19"/>
+      <c r="I1543" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1544" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1544" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1544" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1544" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1544" s="19" t="s">
+        <v>1984</v>
+      </c>
+      <c r="F1544" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1544" s="19">
+        <v>254</v>
+      </c>
+      <c r="H1544" s="19"/>
+      <c r="I1544" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1545" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1545" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1545" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1545" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1545" s="19" t="s">
+        <v>1985</v>
+      </c>
+      <c r="F1545" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1545" s="19">
+        <v>4</v>
+      </c>
+      <c r="H1545" s="19"/>
+      <c r="I1545" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1546" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1546" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1546" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1546" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1546" s="19" t="s">
+        <v>1986</v>
+      </c>
+      <c r="F1546" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1546" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1546" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1546" t="s">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1547" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1547" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1547" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1547" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1547" s="19" t="s">
+        <v>1987</v>
+      </c>
+      <c r="F1547" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1547" s="19">
+        <v>22</v>
+      </c>
+      <c r="H1547" s="19">
+        <v>0</v>
+      </c>
+      <c r="I1547" t="s">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1548" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1548" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1548" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1548" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1548" s="19" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F1548" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1548" s="19">
+        <v>1</v>
+      </c>
+      <c r="H1548" s="19"/>
+      <c r="I1548" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1549" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1549" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1549" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1549" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1549" s="19" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F1549" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1549" s="19">
+        <v>7</v>
+      </c>
+      <c r="H1549" s="19"/>
+      <c r="I1549" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1550" s="4">
+        <v>43368</v>
+      </c>
+      <c r="B1550" s="6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C1550" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1550" s="19" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E1550" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1550" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1550" s="19">
+        <v>19</v>
+      </c>
+      <c r="H1550" s="19"/>
+      <c r="I1550" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1552" s="23" t="s">
+        <v>2001</v>
+      </c>
+      <c r="E1552" s="24"/>
+      <c r="F1552" s="24"/>
+      <c r="G1552" s="24"/>
+      <c r="H1552" s="24"/>
+      <c r="I1552" s="24"/>
+    </row>
+    <row r="1553" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D1553" s="24"/>
+      <c r="E1553" s="24"/>
+      <c r="F1553" s="24"/>
+      <c r="G1553" s="24"/>
+      <c r="H1553" s="24"/>
+      <c r="I1553" s="24"/>
+    </row>
+    <row r="1554" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D1554" s="24"/>
+      <c r="E1554" s="24"/>
+      <c r="F1554" s="24"/>
+      <c r="G1554" s="24"/>
+      <c r="H1554" s="24"/>
+      <c r="I1554" s="24"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{F4AE1B9E-5266-4134-A2C3-A4E39633C052}" topLeftCell="C1">
@@ -43054,7 +43838,41 @@
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="49">
+  <mergeCells count="50">
+    <mergeCell ref="D1552:I1554"/>
+    <mergeCell ref="D17:L19"/>
+    <mergeCell ref="D68:L70"/>
+    <mergeCell ref="D113:L115"/>
+    <mergeCell ref="D335:L337"/>
+    <mergeCell ref="D603:I605"/>
+    <mergeCell ref="D502:I504"/>
+    <mergeCell ref="D449:I451"/>
+    <mergeCell ref="D466:I468"/>
+    <mergeCell ref="D485:I487"/>
+    <mergeCell ref="D562:I564"/>
+    <mergeCell ref="D524:L526"/>
+    <mergeCell ref="D363:I365"/>
+    <mergeCell ref="D92:I94"/>
+    <mergeCell ref="D1484:I1486"/>
+    <mergeCell ref="D613:I615"/>
+    <mergeCell ref="D629:I631"/>
+    <mergeCell ref="D648:I650"/>
+    <mergeCell ref="D665:I667"/>
+    <mergeCell ref="D693:I695"/>
+    <mergeCell ref="D1346:L1348"/>
+    <mergeCell ref="D1361:L1363"/>
+    <mergeCell ref="D1386:L1388"/>
+    <mergeCell ref="D1292:L1294"/>
+    <mergeCell ref="D1236:L1238"/>
+    <mergeCell ref="D1129:I1131"/>
+    <mergeCell ref="D1267:L1269"/>
+    <mergeCell ref="D1421:L1423"/>
+    <mergeCell ref="D1431:L1433"/>
+    <mergeCell ref="D143:I145"/>
+    <mergeCell ref="D295:I297"/>
+    <mergeCell ref="D318:I320"/>
+    <mergeCell ref="D244:I246"/>
+    <mergeCell ref="D199:I201"/>
     <mergeCell ref="D1252:L1254"/>
     <mergeCell ref="D1522:I1524"/>
     <mergeCell ref="D835:I837"/>
@@ -43071,39 +43889,6 @@
     <mergeCell ref="D1468:I1470"/>
     <mergeCell ref="D1309:L1311"/>
     <mergeCell ref="D1326:L1328"/>
-    <mergeCell ref="D1431:L1433"/>
-    <mergeCell ref="D143:I145"/>
-    <mergeCell ref="D295:I297"/>
-    <mergeCell ref="D318:I320"/>
-    <mergeCell ref="D244:I246"/>
-    <mergeCell ref="D1484:I1486"/>
-    <mergeCell ref="D613:I615"/>
-    <mergeCell ref="D629:I631"/>
-    <mergeCell ref="D648:I650"/>
-    <mergeCell ref="D665:I667"/>
-    <mergeCell ref="D693:I695"/>
-    <mergeCell ref="D1346:L1348"/>
-    <mergeCell ref="D1361:L1363"/>
-    <mergeCell ref="D1386:L1388"/>
-    <mergeCell ref="D1292:L1294"/>
-    <mergeCell ref="D1236:L1238"/>
-    <mergeCell ref="D1129:I1131"/>
-    <mergeCell ref="D199:I201"/>
-    <mergeCell ref="D1267:L1269"/>
-    <mergeCell ref="D1421:L1423"/>
-    <mergeCell ref="D17:L19"/>
-    <mergeCell ref="D68:L70"/>
-    <mergeCell ref="D113:L115"/>
-    <mergeCell ref="D335:L337"/>
-    <mergeCell ref="D603:I605"/>
-    <mergeCell ref="D502:I504"/>
-    <mergeCell ref="D449:I451"/>
-    <mergeCell ref="D466:I468"/>
-    <mergeCell ref="D485:I487"/>
-    <mergeCell ref="D562:I564"/>
-    <mergeCell ref="D524:L526"/>
-    <mergeCell ref="D363:I365"/>
-    <mergeCell ref="D92:I94"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -43120,7 +43905,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43196,8 +43981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43939,8 +44724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44152,7 +44937,7 @@
         <v>1398</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>874</v>
+        <v>1709</v>
       </c>
       <c r="C15" s="21" t="s">
         <v>1490</v>
@@ -50671,8 +51456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53174,15 +53959,49 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
-      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
-      <Description>STHNKY6CXN64-585-23125</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53331,49 +54150,15 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">STHNKY6CXN64-585-23125</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d">
+      <Url>https://connect.ufl.edu/it/Projects/83804A/_layouts/DocIdRedir.aspx?ID=STHNKY6CXN64-585-23125</Url>
+      <Description>STHNKY6CXN64-585-23125</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53385,17 +54170,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02EC59C-3037-4324-9F25-70F5C5DE4AE3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDFF90A1-0238-4E08-AF86-38ADE0A38CA8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -53419,9 +54196,17 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDFF90A1-0238-4E08-AF86-38ADE0A38CA8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02EC59C-3037-4324-9F25-70F5C5DE4AE3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3cfd9aaa-4fb7-4c22-8109-d679e3e9d77d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>